<commit_message>
replacing spreadsheet with one that includes the garage geometry tags
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-2st-garage/model_geometry_with_garage.xlsx
+++ b/OptFramework/GenericHome-2st-garage/model_geometry_with_garage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6015" windowWidth="19230" windowHeight="6060"/>
+    <workbookView xWindow="-15" yWindow="6015" windowWidth="19230" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry options" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <definedName name="AreaWinWall4Ratio">'geometry calculation'!$H$15</definedName>
     <definedName name="FloorAreaPerStorey">'Geometry options'!$E$3</definedName>
     <definedName name="found_wall_area" localSheetId="3">'geometry calculation-original'!$I$21</definedName>
-    <definedName name="found_wall_area">'geometry calculation'!$I$22</definedName>
+    <definedName name="found_wall_area">'geometry calculation'!$I$26</definedName>
     <definedName name="Hght_Flr1" localSheetId="3">'geometry calculation-original'!$C$8</definedName>
     <definedName name="Hght_Flr1" comment="Height of floor 1 (ground floor)">'geometry calculation'!$C$10</definedName>
     <definedName name="Hght_Flr2" localSheetId="3">'geometry calculation-original'!$C$9</definedName>
@@ -81,7 +81,7 @@
     <definedName name="Len_WinWall4">'geometry calculation'!$M$15</definedName>
     <definedName name="Length">'Geometry options'!$G$3</definedName>
     <definedName name="main_area" localSheetId="3">'geometry calculation-original'!$I$18</definedName>
-    <definedName name="main_area">'geometry calculation'!$I$19</definedName>
+    <definedName name="main_area">'geometry calculation'!$I$23</definedName>
     <definedName name="NumberStoreys">'Geometry options'!$D$3</definedName>
     <definedName name="NumStorey">'Geometry options'!$D$4</definedName>
     <definedName name="NumStoreys" localSheetId="3">'geometry calculation-original'!$C$4</definedName>
@@ -103,50 +103,50 @@
     <definedName name="Roof_Slope1" localSheetId="3">'geometry calculation-original'!$H$16</definedName>
     <definedName name="Roof_Slope1">'geometry calculation'!$C$16</definedName>
     <definedName name="second_area" localSheetId="3">'geometry calculation-original'!$I$19</definedName>
-    <definedName name="second_area">'geometry calculation'!$I$20</definedName>
+    <definedName name="second_area">'geometry calculation'!$I$24</definedName>
     <definedName name="third_area" localSheetId="3">'geometry calculation-original'!$I$20</definedName>
-    <definedName name="third_area">'geometry calculation'!$I$21</definedName>
+    <definedName name="third_area">'geometry calculation'!$I$25</definedName>
     <definedName name="Total_area">'Geometry options'!$C$3</definedName>
-    <definedName name="total_window_area">'geometry calculation'!$I$23</definedName>
+    <definedName name="total_window_area">'geometry calculation'!$I$27</definedName>
     <definedName name="Width">'Geometry options'!$F$3</definedName>
     <definedName name="win_bottom" localSheetId="3">'geometry calculation-original'!$C$15</definedName>
     <definedName name="win_bottom">'geometry calculation'!#REF!</definedName>
     <definedName name="win_top" localSheetId="3">'geometry calculation-original'!$C$16</definedName>
     <definedName name="win_top">'geometry calculation'!#REF!</definedName>
     <definedName name="win_wall_1_left" localSheetId="3">'geometry calculation-original'!$C$18</definedName>
-    <definedName name="win_wall_1_left">'geometry calculation'!$C$20</definedName>
+    <definedName name="win_wall_1_left">'geometry calculation'!$C$24</definedName>
     <definedName name="win_wall_1_right" localSheetId="3">'geometry calculation-original'!$C$17</definedName>
-    <definedName name="win_wall_1_right">'geometry calculation'!$C$19</definedName>
+    <definedName name="win_wall_1_right">'geometry calculation'!$C$23</definedName>
     <definedName name="win_wall_2_left" localSheetId="3">'geometry calculation-original'!$C$20</definedName>
-    <definedName name="win_wall_2_left">'geometry calculation'!$C$22</definedName>
+    <definedName name="win_wall_2_left">'geometry calculation'!$C$26</definedName>
     <definedName name="win_wall_2_right" localSheetId="3">'geometry calculation-original'!$C$19</definedName>
-    <definedName name="win_wall_2_right">'geometry calculation'!$C$21</definedName>
+    <definedName name="win_wall_2_right">'geometry calculation'!$C$25</definedName>
     <definedName name="win_wall_3_left" localSheetId="3">'geometry calculation-original'!$C$22</definedName>
-    <definedName name="win_wall_3_left">'geometry calculation'!$C$24</definedName>
+    <definedName name="win_wall_3_left">'geometry calculation'!$C$28</definedName>
     <definedName name="win_wall_3_right" localSheetId="3">'geometry calculation-original'!$C$21</definedName>
-    <definedName name="win_wall_3_right">'geometry calculation'!$C$23</definedName>
+    <definedName name="win_wall_3_right">'geometry calculation'!$C$27</definedName>
     <definedName name="win_wall_4_left" localSheetId="3">'geometry calculation-original'!$C$24</definedName>
-    <definedName name="win_wall_4_left">'geometry calculation'!$C$26</definedName>
+    <definedName name="win_wall_4_left">'geometry calculation'!$C$30</definedName>
     <definedName name="win_wall_4_right" localSheetId="3">'geometry calculation-original'!$C$23</definedName>
-    <definedName name="win_wall_4_right">'geometry calculation'!$C$25</definedName>
+    <definedName name="win_wall_4_right">'geometry calculation'!$C$29</definedName>
     <definedName name="x1st" localSheetId="3">'geometry calculation-original'!$B$28:$B$51</definedName>
-    <definedName name="x1st" comment="x-coordinates for all vertices">'geometry calculation'!$B$32:$B$55</definedName>
+    <definedName name="x1st" comment="x-coordinates for all vertices">'geometry calculation'!$B$36:$B$59</definedName>
     <definedName name="x2nd" localSheetId="3">'geometry calculation-original'!$F$28:$F$51</definedName>
-    <definedName name="x2nd">'geometry calculation'!$F$32:$F$55</definedName>
+    <definedName name="x2nd">'geometry calculation'!$F$36:$F$59</definedName>
     <definedName name="x3rd" localSheetId="3">'geometry calculation-original'!$J$28:$J$51</definedName>
-    <definedName name="x3rd">'geometry calculation'!$J$32:$J$55</definedName>
+    <definedName name="x3rd">'geometry calculation'!$J$36:$J$59</definedName>
     <definedName name="y1st" localSheetId="3">'geometry calculation-original'!$C$28:$C$51</definedName>
-    <definedName name="y1st" comment="y-coordinates of all vertices">'geometry calculation'!$C$32:$C$55</definedName>
+    <definedName name="y1st" comment="y-coordinates of all vertices">'geometry calculation'!$C$36:$C$59</definedName>
     <definedName name="y2nd" localSheetId="3">'geometry calculation-original'!$G$28:$G$51</definedName>
-    <definedName name="y2nd">'geometry calculation'!$G$32:$G$55</definedName>
+    <definedName name="y2nd">'geometry calculation'!$G$36:$G$59</definedName>
     <definedName name="y3rd" localSheetId="3">'geometry calculation-original'!$K$28:$K$51</definedName>
-    <definedName name="y3rd">'geometry calculation'!$K$32:$K$55</definedName>
+    <definedName name="y3rd">'geometry calculation'!$K$36:$K$59</definedName>
     <definedName name="z1st" localSheetId="3">'geometry calculation-original'!$D$28:$D$51</definedName>
-    <definedName name="z1st" comment="z-coordinates of all vertices">'geometry calculation'!$D$32:$D$55</definedName>
+    <definedName name="z1st" comment="z-coordinates of all vertices">'geometry calculation'!$D$36:$D$59</definedName>
     <definedName name="z2nd" localSheetId="3">'geometry calculation-original'!$H$28:$H$51</definedName>
-    <definedName name="z2nd" comment="z-coordinates for the 2storey of house, if applicable">'geometry calculation'!$H$32:$H$55</definedName>
+    <definedName name="z2nd" comment="z-coordinates for the 2storey of house, if applicable">'geometry calculation'!$H$36:$H$59</definedName>
     <definedName name="z3rd" localSheetId="3">'geometry calculation-original'!$L$28:$L$51</definedName>
-    <definedName name="z3rd">'geometry calculation'!$L$32:$L$55</definedName>
+    <definedName name="z3rd">'geometry calculation'!$L$36:$L$59</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
@@ -192,41 +192,6 @@
     <author>Purdy, Julia</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Purdy, Julia:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Must be the larger of the two dimensions
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Purdy, Julia</author>
-  </authors>
-  <commentList>
     <comment ref="C6" authorId="0">
       <text>
         <r>
@@ -257,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="191">
   <si>
     <t>m²</t>
   </si>
@@ -799,7 +764,37 @@
     <t>Base Case for Lighthouse retrofit analysis. Based on EGH database vancouver 1980</t>
   </si>
   <si>
-    <t>Vancouver_new_3storey_semi</t>
+    <t>Garage</t>
+  </si>
+  <si>
+    <t>Inset Garage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garage </t>
+  </si>
+  <si>
+    <t>&lt;gar-width&gt;</t>
+  </si>
+  <si>
+    <t>&lt;gar-length&gt;</t>
+  </si>
+  <si>
+    <t>&lt;gar-area&gt;</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Vancouver_new_3storey_semi_garage</t>
+  </si>
+  <si>
+    <t>Vancouver_new_2storey_row_garage</t>
+  </si>
+  <si>
+    <t>NZEH-Arch</t>
   </si>
 </sst>
 </file>
@@ -995,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1176,11 +1171,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1191,9 +1198,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1713,15 +1717,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S7"/>
+  <dimension ref="B1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="47" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="47" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="47" customWidth="1"/>
@@ -1733,20 +1738,24 @@
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="19.28515625" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="12.28515625" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="H1" s="92" t="s">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H1" s="94" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-    </row>
-    <row r="2" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="S1" s="95" t="s">
+        <v>182</v>
+      </c>
+      <c r="T1" s="95"/>
+    </row>
+    <row r="2" spans="2:21" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>146</v>
       </c>
@@ -1798,11 +1807,17 @@
       <c r="R2" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="S2" s="70" t="s">
+      <c r="S2" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="T2" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="U2" s="70" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>149</v>
       </c>
@@ -1820,7 +1835,7 @@
         <v>11.5</v>
       </c>
       <c r="G3" s="66">
-        <f>+E3/F3</f>
+        <f t="shared" ref="G3:G9" si="0">+E3/F3</f>
         <v>11.491304347826087</v>
       </c>
       <c r="H3" s="47">
@@ -1859,11 +1874,13 @@
       <c r="R3" s="85">
         <v>2</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>153</v>
       </c>
@@ -1881,7 +1898,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="66">
-        <f>+E4/F4</f>
+        <f t="shared" si="0"/>
         <v>9.2592592592592595</v>
       </c>
       <c r="H4" s="66">
@@ -1917,8 +1934,10 @@
       <c r="R4" s="85">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>154</v>
       </c>
@@ -1936,7 +1955,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="47">
-        <f>+E5/F5</f>
+        <f t="shared" si="0"/>
         <v>9.5100000000000016</v>
       </c>
       <c r="H5" s="47">
@@ -1973,8 +1992,10 @@
       <c r="R5" s="85">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>177</v>
       </c>
@@ -1993,7 +2014,7 @@
         <v>12.9</v>
       </c>
       <c r="G6" s="68">
-        <f>+E6/F6</f>
+        <f t="shared" si="0"/>
         <v>8.6344413705656891</v>
       </c>
       <c r="H6" s="87">
@@ -2032,56 +2053,201 @@
       <c r="R6" s="88">
         <v>1.9</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="88"/>
+      <c r="T6" s="88"/>
+      <c r="U6" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C7" s="47">
-        <v>176.5</v>
+        <v>167.5</v>
       </c>
       <c r="D7" s="47">
         <v>3</v>
       </c>
       <c r="E7" s="86">
         <f>+C7/D7</f>
-        <v>58.833333333333336</v>
+        <v>55.833333333333336</v>
       </c>
       <c r="F7" s="47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G7" s="47">
-        <f>+E7/F7</f>
-        <v>8.4047619047619051</v>
+        <f t="shared" si="0"/>
+        <v>11.166666666666668</v>
       </c>
       <c r="H7" s="87">
-        <f>100*10.32/56.9</f>
-        <v>18.13708260105448</v>
+        <v>10</v>
       </c>
       <c r="I7" s="87">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J7" s="87">
-        <f>100*17/66.99</f>
-        <v>25.37692192864607</v>
+        <v>20</v>
       </c>
       <c r="K7" s="87">
-        <f>100*2.68/63.28</f>
-        <v>4.2351453855878631</v>
-      </c>
-      <c r="L7" s="90">
-        <v>0.66700000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="L7" s="68">
+        <f>3/12</f>
+        <v>0.25</v>
       </c>
       <c r="M7" s="47">
         <v>2.2999999999999998</v>
       </c>
+      <c r="N7" s="88">
+        <v>3.048</v>
+      </c>
+      <c r="O7" s="88">
+        <v>2.44</v>
+      </c>
+      <c r="P7" s="88">
+        <v>2.44</v>
+      </c>
+      <c r="Q7" s="88">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="R7" s="88">
+        <v>1.9</v>
+      </c>
+      <c r="S7" s="88">
+        <v>3.3018999999999998</v>
+      </c>
+      <c r="T7" s="88">
+        <v>3.5051999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="92">
+        <v>125</v>
+      </c>
+      <c r="D8" s="92">
+        <v>2</v>
+      </c>
+      <c r="E8" s="86">
+        <f>+C8/D8</f>
+        <v>62.5</v>
+      </c>
+      <c r="F8" s="92">
+        <v>5</v>
+      </c>
+      <c r="G8" s="92">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="H8" s="87">
+        <v>10</v>
+      </c>
+      <c r="I8" s="87">
+        <v>5</v>
+      </c>
+      <c r="J8" s="87">
+        <v>20</v>
+      </c>
+      <c r="K8" s="87">
+        <v>1</v>
+      </c>
+      <c r="L8" s="68">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="M8" s="92">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N8" s="88">
+        <v>3.048</v>
+      </c>
+      <c r="O8" s="88">
+        <v>2.44</v>
+      </c>
+      <c r="P8" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="88">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="R8" s="88">
+        <v>1.9</v>
+      </c>
+      <c r="S8" s="88">
+        <v>3.3018999999999998</v>
+      </c>
+      <c r="T8" s="88">
+        <v>3.5051999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="86">
+        <f>2396.99/10.76</f>
+        <v>222.76858736059478</v>
+      </c>
+      <c r="D9" s="47">
+        <v>2</v>
+      </c>
+      <c r="E9" s="86">
+        <f>+C9/D9</f>
+        <v>111.38429368029739</v>
+      </c>
+      <c r="F9" s="47">
+        <v>12.9</v>
+      </c>
+      <c r="G9" s="68">
+        <f t="shared" si="0"/>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H9" s="47">
+        <v>18</v>
+      </c>
+      <c r="I9" s="47">
+        <v>0</v>
+      </c>
+      <c r="J9" s="47">
+        <v>25</v>
+      </c>
+      <c r="K9" s="47">
+        <v>4</v>
+      </c>
+      <c r="L9" s="93">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M9" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="N9" s="88">
+        <v>2.79</v>
+      </c>
+      <c r="O9" s="88">
+        <v>2.44</v>
+      </c>
+      <c r="P9" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="88">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="R9" s="88">
+        <v>1.9</v>
+      </c>
+      <c r="S9" s="88"/>
+      <c r="T9" s="88"/>
+      <c r="U9" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H1:K1"/>
+    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2090,17 +2256,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:T59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
@@ -2117,7 +2283,7 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="F2" s="59"/>
       <c r="G2" s="59"/>
@@ -2148,7 +2314,7 @@
       <c r="D4" s="1"/>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
-      <c r="H4" s="94" t="s">
+      <c r="H4" s="98" t="s">
         <v>89</v>
       </c>
       <c r="I4" s="58" t="s">
@@ -2167,8 +2333,8 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="64">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,2,FALSE)</f>
-        <v>264.3</v>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:U38,2,FALSE)</f>
+        <v>222.76858736059478</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -2179,12 +2345,12 @@
       <c r="G5" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="95"/>
-      <c r="I5" s="93" t="s">
+      <c r="H5" s="99"/>
+      <c r="I5" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2192,7 +2358,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="64">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,3,FALSE)</f>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:U38,3,FALSE)</f>
         <v>2</v>
       </c>
       <c r="D6" s="1"/>
@@ -2204,11 +2370,11 @@
       </c>
       <c r="I6" s="33">
         <f>+(INDEX(x1st,2)-INDEX(x1st,1))*(INDEX(z1st,7)-INDEX(z1st,2))</f>
-        <v>35.051999999999992</v>
+        <v>35.991000000000007</v>
       </c>
       <c r="J6" s="33">
         <f>+(INDEX(x2nd,2)-INDEX(x2nd,1))*(INDEX(z2nd,7)-INDEX(z2nd,2))</f>
-        <v>28.059999999999995</v>
+        <v>31.475999999999996</v>
       </c>
       <c r="K6" s="33">
         <f>+(INDEX(x3rd,2)-INDEX(x3rd,1))*(INDEX(z3rd,7)-INDEX(z3rd,2))</f>
@@ -2226,8 +2392,8 @@
         <v>6</v>
       </c>
       <c r="C7" s="11">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,4,FALSE)</f>
-        <v>132.15</v>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:U38,4,FALSE)</f>
+        <v>111.38429368029739</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>0</v>
@@ -2240,11 +2406,11 @@
       </c>
       <c r="I7" s="33">
         <f>+(INDEX(y1st,3)-INDEX(y1st,2))*(INDEX(z1st,7)-(INDEX(z1st,3)))</f>
-        <v>35.025495652173909</v>
+        <v>24.090091423878278</v>
       </c>
       <c r="J7" s="33">
         <f>+(INDEX(y2nd,3)-INDEX(y2nd,2))*(INDEX(z2nd,7)-(INDEX(z2nd,3)))</f>
-        <v>28.038782608695648</v>
+        <v>21.068036944180278</v>
       </c>
       <c r="K7" s="33">
         <f>+(INDEX(y3rd,3)-INDEX(y3rd,2))*(INDEX(z3rd,7)-(INDEX(z3rd,3)))</f>
@@ -2262,8 +2428,8 @@
         <v>80</v>
       </c>
       <c r="C8" s="76">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,5,FALSE)</f>
-        <v>11.5</v>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:U38,5,FALSE)</f>
+        <v>12.9</v>
       </c>
       <c r="D8" s="39" t="s">
         <v>1</v>
@@ -2276,11 +2442,11 @@
       </c>
       <c r="I8" s="33">
         <f>(INDEX(x1st,3)-INDEX(x1st,4))*(INDEX(z1st,7)-INDEX(z1st,4))</f>
-        <v>35.051999999999992</v>
+        <v>35.991000000000007</v>
       </c>
       <c r="J8" s="33">
         <f>(INDEX(x2nd,3)-INDEX(x2nd,4))*(INDEX(z2nd,7)-INDEX(z2nd,4))</f>
-        <v>28.059999999999995</v>
+        <v>31.475999999999996</v>
       </c>
       <c r="K8" s="33">
         <f>(INDEX(x3rd,3)-INDEX(x3rd,4))*(INDEX(z3rd,7)-INDEX(z3rd,4))</f>
@@ -2298,8 +2464,8 @@
         <v>81</v>
       </c>
       <c r="C9" s="76">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,6,FALSE)</f>
-        <v>11.491304347826087</v>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:U38,6,FALSE)</f>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>1</v>
@@ -2313,11 +2479,11 @@
       </c>
       <c r="I9" s="33">
         <f>(INDEX(y1st,4)-INDEX(y1st,1))*(INDEX(z1st,8)-INDEX(z1st,4))</f>
-        <v>35.025495652173909</v>
+        <v>24.090091423878278</v>
       </c>
       <c r="J9" s="33">
         <f>(INDEX(y2nd,4)-INDEX(y2nd,1))*(INDEX(z2nd,8)-INDEX(z2nd,4))</f>
-        <v>28.038782608695648</v>
+        <v>21.068036944180278</v>
       </c>
       <c r="K9" s="33">
         <f>(INDEX(y3rd,4)-INDEX(y3rd,1))*(INDEX(z3rd,8)-INDEX(z3rd,4))</f>
@@ -2333,8 +2499,8 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="76">
-        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,13,FALSE)</f>
-        <v>3.048</v>
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,13,FALSE)</f>
+        <v>2.79</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -2347,15 +2513,15 @@
       </c>
       <c r="I10" s="33">
         <f>INDEX(x1st,6)*INDEX(y1st,7)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="J10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="K10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="L10" t="s">
         <v>0</v>
@@ -2367,7 +2533,7 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="76">
-        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,14,FALSE)</f>
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,14,FALSE)</f>
         <v>2.44</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2381,15 +2547,15 @@
       </c>
       <c r="I11" s="33">
         <f>INDEX(x1st,3)*INDEX(y1st,4)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="J11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="K11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="L11" t="s">
         <v>0</v>
@@ -2407,7 +2573,7 @@
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="76">
-        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,15,FALSE)</f>
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,15,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2421,15 +2587,15 @@
       </c>
       <c r="H12" s="43">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,7,FALSE)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I12" s="15">
         <f>AreaWall1*AreaWinWall1Ratio/100</f>
-        <v>5.2577999999999987</v>
+        <v>6.4783800000000005</v>
       </c>
       <c r="J12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>4.2089999999999996</v>
+        <v>5.6656799999999983</v>
       </c>
       <c r="K12" s="15">
         <f>+IF(NumStoreys=3,AreaWall1_2nd*AreaWinWall1Ratio/100,0)</f>
@@ -2440,15 +2606,15 @@
       </c>
       <c r="M12" s="27">
         <f>AreaWinWall1/Hght_WinWall1</f>
-        <v>3.4499999999999997</v>
+        <v>4.6439999999999992</v>
       </c>
       <c r="N12" s="26">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O12">
         <f>+Len_WinWall1*Hght_WinWall1</f>
-        <v>5.2577999999999987</v>
+        <v>6.4783800000000005</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2457,7 +2623,7 @@
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="76">
-        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,16,FALSE)</f>
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,16,FALSE)</f>
         <v>2.4384000000000001</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2471,15 +2637,15 @@
       </c>
       <c r="H13" s="44">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,8,FALSE)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I13" s="17">
         <f>AreaWall2*AreaWinWall2Ratio/100</f>
-        <v>5.253824347826086</v>
+        <v>0</v>
       </c>
       <c r="J13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>4.2058173913043468</v>
+        <v>0</v>
       </c>
       <c r="K13" s="17">
         <f>+IF(NumStoreys=3,AreaWall2_2nd*AreaWinWall2Ratio/100,0)</f>
@@ -2490,15 +2656,15 @@
       </c>
       <c r="M13" s="28">
         <f>AreaWinWall2/Hght_WinWall2</f>
-        <v>3.4473913043478257</v>
+        <v>0</v>
       </c>
       <c r="N13" s="29">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O13">
         <f>+Len_WinWall2*Hght_WinWall2</f>
-        <v>5.253824347826086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2507,8 +2673,8 @@
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="76">
-        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,17,FALSE)</f>
-        <v>2</v>
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,17,FALSE)</f>
+        <v>1.9</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -2521,15 +2687,15 @@
       </c>
       <c r="H14" s="45">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,9,FALSE)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I14" s="18">
         <f>AreaWall3*AreaWinWall3Ratio/100</f>
-        <v>5.2577999999999987</v>
+        <v>8.9977500000000017</v>
       </c>
       <c r="J14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>4.2089999999999996</v>
+        <v>7.8689999999999989</v>
       </c>
       <c r="K14" s="18">
         <f>+IF(NumStoreys=3,AreaWall3_2nd*AreaWinWall3Ratio/100,0)</f>
@@ -2540,15 +2706,15 @@
       </c>
       <c r="M14" s="30">
         <f>AreaWinWall3/Hght_WinWall3</f>
-        <v>3.4499999999999997</v>
+        <v>6.45</v>
       </c>
       <c r="N14" s="31">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O14">
         <f>+Len_WinWall3*Hght_WinWall3</f>
-        <v>5.2577999999999987</v>
+        <v>8.9977500000000017</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2558,7 +2724,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="39">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>49</v>
@@ -2567,16 +2733,15 @@
         <v>53</v>
       </c>
       <c r="H15" s="46">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:O38,10,FALSE)</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I15" s="20">
         <f>AreaWall4*AreaWinWall4Ratio/100</f>
-        <v>5.253824347826086</v>
+        <v>1.204504571193914</v>
       </c>
       <c r="J15" s="20">
         <f>AreaWall4_2nd*AreaWinWall4Ratio/100</f>
-        <v>4.2058173913043468</v>
+        <v>1.0534018472090139</v>
       </c>
       <c r="K15" s="20">
         <f>+IF(NumStoreys=3,AreaWall4_2nd*AreaWinWall4Ratio/100,0)</f>
@@ -2587,15 +2752,15 @@
       </c>
       <c r="M15" s="36">
         <f>AreaWinWall4/Hght_WinWall4</f>
-        <v>3.4473913043478257</v>
+        <v>0.86344413705656897</v>
       </c>
       <c r="N15" s="32">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O15">
         <f>+Len_WinWall4*Hght_WinWall4</f>
-        <v>5.253824347826086</v>
+        <v>1.204504571193914</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2605,7 +2770,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="74">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,11,FALSE)</f>
-        <v>0.25</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2617,14 +2782,14 @@
       <c r="M16" s="78"/>
       <c r="N16" s="79"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="7" t="s">
         <v>162</v>
       </c>
       <c r="C17" s="35">
         <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Roof_Peak_W*Roof_Slope1)</f>
-        <v>9.3638999999999992</v>
+        <v>11.970549999999999</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -2639,1368 +2804,1496 @@
       <c r="M17" s="78"/>
       <c r="N17" s="79"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C18" s="11">
         <f>Opt_Width/2</f>
-        <v>5.75</v>
+        <v>6.45</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="11">
+        <f>VLOOKUP($B$2,'Geometry options'!B3:U38,18,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="11">
+        <f>VLOOKUP($B$2,'Geometry options'!B4:U39,19,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" s="11">
+        <f>+C19*C20</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C23" s="14">
         <f>INDEX(x1st,9)</f>
         <v>0.5</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F23" t="s">
         <v>134</v>
       </c>
-      <c r="I19" s="42">
+      <c r="I23" s="42">
         <f>SUM(I6:I9)-SUM(I12:I15)</f>
-        <v>119.13174260869562</v>
-      </c>
-      <c r="J19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+        <v>103.48154827656265</v>
+      </c>
+      <c r="J23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C24" s="15">
         <f>INDEX(x1st,10)</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="F20" t="s">
+        <v>5.1439999999999992</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="F24" t="s">
         <v>137</v>
       </c>
-      <c r="I20" s="91">
+      <c r="I24" s="90">
         <f>+SUM(J6:J9)-SUM(J12:J15)</f>
-        <v>95.367930434782593</v>
-      </c>
-      <c r="J20" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4" t="s">
+        <v>90.499992041151543</v>
+      </c>
+      <c r="J24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C25" s="16">
         <f>INDEX(y1st,13)</f>
         <v>0.5</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F25" t="s">
         <v>135</v>
       </c>
-      <c r="I21" s="91">
+      <c r="I25" s="90">
         <f>+SUM(K6:K9)-SUM(K12:K15)</f>
         <v>0</v>
       </c>
-      <c r="J21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="4" t="s">
+      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C26" s="17">
         <f>INDEX(y1st,14)</f>
-        <v>3.9473913043478257</v>
-      </c>
-      <c r="F22" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="F26" t="s">
         <v>136</v>
       </c>
-      <c r="I22">
+      <c r="I26">
         <f>2*(Opt_Width*Opt_Bsm_Height)+2*(Opt_Length*Opt_Bsm_Height)</f>
-        <v>112.12399304347827</v>
-      </c>
-      <c r="J22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
+        <v>105.01916367597477</v>
+      </c>
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C27" s="18">
         <f>INDEX(x1st,17)</f>
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
+        <v>12.4</v>
+      </c>
+      <c r="F27" t="s">
         <v>161</v>
       </c>
-      <c r="I23">
+      <c r="I27">
         <f>+AreaWinWall1Ratio/100*SUM(I6:K6)+AreaWinWall2Ratio/100*SUM(I7:K7)+AreaWinWall3Ratio/100*SUM(I8:K8)+AreaWinWall4Ratio/100*SUM(I9:K9)</f>
-        <v>37.852883478260864</v>
-      </c>
-      <c r="J23" t="s">
-        <v>0</v>
-      </c>
-      <c r="K23" s="91">
+        <v>31.268716418402928</v>
+      </c>
+      <c r="J27" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="90">
         <f>+SUM(I12:K15)</f>
-        <v>37.852883478260864</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+        <v>31.268716418402928</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C28" s="18">
         <f>INDEX(x1st,18)</f>
-        <v>7.5500000000000007</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C29" s="19">
         <f>INDEX(y1st,21)</f>
-        <v>10.991304347826087</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+        <v>8.1344413705656891</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C30" s="20">
         <f>INDEX(y1st,22)</f>
-        <v>7.5439130434782617</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="61"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="96" t="s">
+        <v>7.27099723350912</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+      <c r="C33" s="61"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="96"/>
-      <c r="F30" s="96" t="s">
+      <c r="C34" s="96"/>
+      <c r="D34" s="96"/>
+      <c r="F34" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="96"/>
-      <c r="H30" s="96"/>
-      <c r="J30" s="96" t="s">
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="J34" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="96"/>
-      <c r="L30" s="96"/>
-      <c r="N30" s="96" t="s">
+      <c r="K34" s="96"/>
+      <c r="L34" s="96"/>
+      <c r="N34" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="O30" s="96"/>
-      <c r="P30" s="96"/>
-      <c r="R30" s="96" t="s">
+      <c r="O34" s="96"/>
+      <c r="P34" s="96"/>
+      <c r="R34" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="S30" s="96"/>
-      <c r="T30" s="96"/>
-    </row>
-    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="S34" s="96"/>
+      <c r="T34" s="96"/>
+    </row>
+    <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B35" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C35" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D35" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F35" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G35" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="37" t="s">
+      <c r="H35" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="37" t="s">
+      <c r="J35" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="K31" s="37" t="s">
+      <c r="K35" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="L31" s="37" t="s">
+      <c r="L35" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="N31" s="65" t="s">
+      <c r="N35" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="O31" s="65" t="s">
+      <c r="O35" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="P31" s="65" t="s">
+      <c r="P35" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="R31" s="65" t="s">
+      <c r="R35" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="S31" s="65" t="s">
+      <c r="S35" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="T31" s="65" t="s">
+      <c r="T35" s="65" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="24">
-        <v>0</v>
-      </c>
-      <c r="C32" s="24">
-        <v>0</v>
-      </c>
-      <c r="D32" s="57">
+      <c r="B36" s="24">
+        <v>0</v>
+      </c>
+      <c r="C36" s="24">
+        <v>0</v>
+      </c>
+      <c r="D36" s="57">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
-      <c r="F32" s="24">
-        <v>0</v>
-      </c>
-      <c r="G32" s="24">
-        <v>0</v>
-      </c>
-      <c r="H32" s="24">
+      <c r="F36" s="24">
+        <v>0</v>
+      </c>
+      <c r="G36" s="24">
+        <v>0</v>
+      </c>
+      <c r="H36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="J32" s="24">
-        <v>0</v>
-      </c>
-      <c r="K32" s="24">
-        <v>0</v>
-      </c>
-      <c r="L32" s="24">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="J36" s="24">
+        <v>0</v>
+      </c>
+      <c r="K36" s="24">
+        <v>0</v>
+      </c>
+      <c r="L36" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-      <c r="N32" s="24">
-        <v>0</v>
-      </c>
-      <c r="O32" s="24">
-        <v>0</v>
-      </c>
-      <c r="P32" s="24">
+      <c r="N36" s="24">
+        <v>0</v>
+      </c>
+      <c r="O36" s="24">
+        <v>0</v>
+      </c>
+      <c r="P36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="R32" s="24">
-        <v>0</v>
-      </c>
-      <c r="S32" s="24">
-        <v>0</v>
-      </c>
-      <c r="T32" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R36" s="24">
+        <v>0</v>
+      </c>
+      <c r="S36" s="24">
+        <v>0</v>
+      </c>
+      <c r="T36" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B37" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="C33" s="24">
-        <v>0</v>
-      </c>
-      <c r="D33" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="C37" s="24">
+        <v>0</v>
+      </c>
+      <c r="D37" s="24">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F37" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="G33" s="24">
-        <v>0</v>
-      </c>
-      <c r="H33" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="G37" s="24">
+        <v>0</v>
+      </c>
+      <c r="H37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="J33" s="25">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="J37" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="K33" s="24">
-        <v>0</v>
-      </c>
-      <c r="L33" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="K37" s="24">
+        <v>0</v>
+      </c>
+      <c r="L37" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-      <c r="N33" s="25">
+      <c r="N37" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="O33" s="24">
-        <v>0</v>
-      </c>
-      <c r="P33" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="O37" s="24">
+        <v>0</v>
+      </c>
+      <c r="P37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="R33" s="25">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R37" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="S33" s="24">
-        <v>0</v>
-      </c>
-      <c r="T33" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+        <v>12.9</v>
+      </c>
+      <c r="S37" s="24">
+        <v>0</v>
+      </c>
+      <c r="T37" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B38" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="C34" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="C38" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D34" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D38" s="24">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F38" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="G34" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="G38" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H34" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="J34" s="25">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="J38" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="K34" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="K38" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L34" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L38" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="25">
+      <c r="N38" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="O34" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="O38" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="P34" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="R34" s="25">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R38" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="S34" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="S38" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="T34" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T38" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="24">
-        <v>0</v>
-      </c>
-      <c r="C35" s="24">
+      <c r="B39" s="24">
+        <v>0</v>
+      </c>
+      <c r="C39" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D35" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D39" s="24">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
-      <c r="F35" s="24">
-        <v>0</v>
-      </c>
-      <c r="G35" s="24">
+      <c r="F39" s="24">
+        <v>0</v>
+      </c>
+      <c r="G39" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H35" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="J35" s="24">
-        <v>0</v>
-      </c>
-      <c r="K35" s="24">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="J39" s="24">
+        <v>0</v>
+      </c>
+      <c r="K39" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L35" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L39" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-      <c r="N35" s="24">
-        <v>0</v>
-      </c>
-      <c r="O35" s="24">
+      <c r="N39" s="24">
+        <v>0</v>
+      </c>
+      <c r="O39" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="P35" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="R35" s="24">
-        <v>0</v>
-      </c>
-      <c r="S35" s="24">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R39" s="24">
+        <v>0</v>
+      </c>
+      <c r="S39" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="T35" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T39" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="24">
-        <v>0</v>
-      </c>
-      <c r="C36" s="24">
-        <v>0</v>
-      </c>
-      <c r="D36" s="24">
+      <c r="B40" s="24">
+        <v>0</v>
+      </c>
+      <c r="C40" s="24">
+        <v>0</v>
+      </c>
+      <c r="D40" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="F36" s="24">
-        <v>0</v>
-      </c>
-      <c r="G36" s="24">
-        <v>0</v>
-      </c>
-      <c r="H36" s="24">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="F40" s="24">
+        <v>0</v>
+      </c>
+      <c r="G40" s="24">
+        <v>0</v>
+      </c>
+      <c r="H40" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="J36" s="24">
-        <v>0</v>
-      </c>
-      <c r="K36" s="24">
-        <v>0</v>
-      </c>
-      <c r="L36" s="24">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="J40" s="24">
+        <v>0</v>
+      </c>
+      <c r="K40" s="24">
+        <v>0</v>
+      </c>
+      <c r="L40" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-      <c r="N36" s="25">
+      <c r="N40" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>5.75</v>
-      </c>
-      <c r="O36" s="24">
-        <v>0</v>
-      </c>
-      <c r="P36" s="24">
+        <v>6.45</v>
+      </c>
+      <c r="O40" s="24">
+        <v>0</v>
+      </c>
+      <c r="P40" s="24">
         <f>+C17</f>
-        <v>9.3638999999999992</v>
-      </c>
-      <c r="R36" s="24">
-        <v>0</v>
-      </c>
-      <c r="S36" s="24">
-        <v>0</v>
-      </c>
-      <c r="T36" s="57">
+        <v>11.970549999999999</v>
+      </c>
+      <c r="R40" s="24">
+        <v>0</v>
+      </c>
+      <c r="S40" s="24">
+        <v>0</v>
+      </c>
+      <c r="T40" s="57">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B41" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="C37" s="24">
-        <v>0</v>
-      </c>
-      <c r="D37" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="C41" s="24">
+        <v>0</v>
+      </c>
+      <c r="D41" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="F37" s="25">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="F41" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="G37" s="24">
-        <v>0</v>
-      </c>
-      <c r="H37" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="G41" s="24">
+        <v>0</v>
+      </c>
+      <c r="H41" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="J37" s="25">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="J41" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="K37" s="24">
-        <v>0</v>
-      </c>
-      <c r="L37" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="K41" s="24">
+        <v>0</v>
+      </c>
+      <c r="L41" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-      <c r="N37" s="25">
+      <c r="N41" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>5.75</v>
-      </c>
-      <c r="O37" s="24">
+        <v>6.45</v>
+      </c>
+      <c r="O41" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="P37" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P41" s="24">
         <f>+C17</f>
-        <v>9.3638999999999992</v>
-      </c>
-      <c r="R37" s="25">
+        <v>11.970549999999999</v>
+      </c>
+      <c r="R41" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="S37" s="24">
-        <v>0</v>
-      </c>
-      <c r="T37" s="57">
+        <v>12.9</v>
+      </c>
+      <c r="S41" s="24">
+        <v>0</v>
+      </c>
+      <c r="T41" s="57">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B42" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="C38" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="C42" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D38" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D42" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="F38" s="25">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="F42" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="G38" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="G42" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H38" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H42" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="J38" s="25">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="J42" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="K38" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="K42" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L38" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L42" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="83"/>
-      <c r="O38" s="84"/>
-      <c r="R38" s="25">
+      <c r="N42" s="83"/>
+      <c r="O42" s="84"/>
+      <c r="R42" s="25">
         <f>Opt_Width</f>
-        <v>11.5</v>
-      </c>
-      <c r="S38" s="24">
+        <v>12.9</v>
+      </c>
+      <c r="S42" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="T38" s="57">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T42" s="57">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="24">
-        <v>0</v>
-      </c>
-      <c r="C39" s="24">
+      <c r="B43" s="24">
+        <v>0</v>
+      </c>
+      <c r="C43" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D39" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D43" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="F39" s="24">
-        <v>0</v>
-      </c>
-      <c r="G39" s="24">
+        <v>5.2284000000000006</v>
+      </c>
+      <c r="F43" s="24">
+        <v>0</v>
+      </c>
+      <c r="G43" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H39" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H43" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
-      </c>
-      <c r="J39" s="24">
-        <v>0</v>
-      </c>
-      <c r="K39" s="24">
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="J43" s="24">
+        <v>0</v>
+      </c>
+      <c r="K43" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L39" s="24">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L43" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-      <c r="N39" s="84"/>
-      <c r="O39" s="84"/>
-      <c r="R39" s="24">
-        <v>0</v>
-      </c>
-      <c r="S39" s="24">
+      <c r="N43" s="84"/>
+      <c r="O43" s="84"/>
+      <c r="R43" s="24">
+        <v>0</v>
+      </c>
+      <c r="S43" s="24">
         <f>Opt_Length</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="T39" s="57">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T43" s="57">
         <f>Opt_Bsm_Height</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="26">
+      <c r="B44" s="26">
         <f>INDEX(x1st,1)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C44" s="26">
         <f>INDEX(y1st,1)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="26">
+      <c r="D44" s="26">
         <f>INDEX(z1st,1)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F40" s="26">
+      <c r="F44" s="26">
         <f>INDEX(x2nd,1)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="G40" s="26">
+      <c r="G44" s="26">
         <f>INDEX(y2nd,1)</f>
         <v>0</v>
       </c>
-      <c r="H40" s="26">
+      <c r="H44" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J40" s="26">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J44" s="26">
         <f>INDEX(x3rd,1)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="K40" s="26">
+      <c r="K44" s="26">
         <f>INDEX(y3rd,1)</f>
         <v>0</v>
       </c>
-      <c r="L40" s="26">
+      <c r="L44" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="27">
+      <c r="B45" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="C41" s="26">
+        <v>5.1439999999999992</v>
+      </c>
+      <c r="C45" s="26">
         <f>INDEX(y1st,2)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D45" s="26">
         <f>INDEX(z1st,1)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F45" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="G41" s="26">
+        <v>5.1439999999999992</v>
+      </c>
+      <c r="G45" s="26">
         <f>INDEX(y2nd,2)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="26">
+      <c r="H45" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J41" s="27">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J45" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="K41" s="26">
+        <v>5.1439999999999992</v>
+      </c>
+      <c r="K45" s="26">
         <f>INDEX(y3rd,2)</f>
         <v>0</v>
       </c>
-      <c r="L41" s="26">
+      <c r="L45" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="N45" s="96" t="s">
+        <v>181</v>
+      </c>
+      <c r="O45" s="96"/>
+      <c r="P45" s="96"/>
+    </row>
+    <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="27">
+      <c r="B46" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="C42" s="26">
+        <v>5.1439999999999992</v>
+      </c>
+      <c r="C46" s="26">
         <f>INDEX(y1st,5)</f>
         <v>0</v>
       </c>
-      <c r="D42" s="26">
+      <c r="D46" s="26">
         <f>INDEX(z1st,9)+Hght_WinWall1</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F42" s="27">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F46" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="G42" s="26">
+        <v>5.1439999999999992</v>
+      </c>
+      <c r="G46" s="26">
         <f>INDEX(y2nd,5)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="26">
+      <c r="H46" s="26">
         <f>INDEX(z2nd,9)+Hght_WinWall1</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J42" s="27">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J46" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="K42" s="26">
+        <v>5.1439999999999992</v>
+      </c>
+      <c r="K46" s="26">
         <f>INDEX(y3rd,5)</f>
         <v>0</v>
       </c>
-      <c r="L42" s="26">
+      <c r="L46" s="26">
         <f>INDEX(z3rd,9)+Hght_WinWall1</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+        <v>1.8950000000000002</v>
+      </c>
+      <c r="N46" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="O46" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="P46" s="91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="26">
+      <c r="B47" s="26">
         <f>INDEX(x1st,9)</f>
         <v>0.5</v>
       </c>
-      <c r="C43" s="26">
+      <c r="C47" s="26">
         <f>INDEX(y1st,6)</f>
         <v>0</v>
       </c>
-      <c r="D43" s="26">
+      <c r="D47" s="26">
         <f>INDEX(z1st,10)+Hght_WinWall1</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F43" s="26">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F47" s="26">
         <f>INDEX(x2nd,9)</f>
         <v>0.5</v>
       </c>
-      <c r="G43" s="26">
+      <c r="G47" s="26">
         <f>INDEX(y2nd,6)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="26">
+      <c r="H47" s="26">
         <f>INDEX(z2nd,10)+Hght_WinWall1</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J43" s="26">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J47" s="26">
         <f>INDEX(x3rd,9)</f>
         <v>0.5</v>
       </c>
-      <c r="K43" s="26">
+      <c r="K47" s="26">
         <f>INDEX(y3rd,6)</f>
         <v>0</v>
       </c>
-      <c r="L43" s="26">
+      <c r="L47" s="26">
         <f>INDEX(z3rd,10)+Hght_WinWall1</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+        <v>1.8950000000000002</v>
+      </c>
+      <c r="N47" s="24">
+        <v>0</v>
+      </c>
+      <c r="O47" s="24">
+        <v>0</v>
+      </c>
+      <c r="P47" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B48" s="28">
         <f>INDEX(x1st,2)</f>
-        <v>11.5</v>
-      </c>
-      <c r="C44" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="C48" s="29">
         <f>INDEX(y1st,2)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D48" s="29">
         <f>INDEX(z1st,2)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F44" s="28">
+      <c r="F48" s="28">
         <f>INDEX(x2nd,2)</f>
-        <v>11.5</v>
-      </c>
-      <c r="G44" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="G48" s="29">
         <f>INDEX(y2nd,2)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="H44" s="29">
+      <c r="H48" s="29">
         <f>INDEX(z2nd,2)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J44" s="28">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J48" s="28">
         <f>INDEX(x3rd,2)</f>
-        <v>11.5</v>
-      </c>
-      <c r="K44" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="K48" s="29">
         <f>INDEX(y3rd,2)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="L44" s="29">
+      <c r="L48" s="29">
         <f>INDEX(z3rd,2)+0.5</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="N48" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="O48" s="24">
+        <v>0</v>
+      </c>
+      <c r="P48" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B49" s="28">
         <f>INDEX(x1st,3)</f>
-        <v>11.5</v>
-      </c>
-      <c r="C45" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="C49" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>3.9473913043478257</v>
-      </c>
-      <c r="D45" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="29">
         <f>INDEX(z1st,3)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F45" s="28">
+      <c r="F49" s="28">
         <f>INDEX(x2nd,3)</f>
-        <v>11.5</v>
-      </c>
-      <c r="G45" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="G49" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>3.9473913043478257</v>
-      </c>
-      <c r="H45" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="H49" s="29">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J45" s="28">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J49" s="28">
         <f>INDEX(x3rd,3)</f>
-        <v>11.5</v>
-      </c>
-      <c r="K45" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="K49" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>3.9473913043478257</v>
-      </c>
-      <c r="L45" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="L49" s="29">
         <f>INDEX(z3rd,3)+0.5</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="N49" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="O49" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P49" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B50" s="28">
         <f>INDEX(x1st,7)</f>
-        <v>11.5</v>
-      </c>
-      <c r="C46" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="C50" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>3.9473913043478257</v>
-      </c>
-      <c r="D46" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="29">
         <f>INDEX(z1st,13)+Hght_WinWall2</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F46" s="28">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F50" s="28">
         <f>INDEX(x2nd,7)</f>
-        <v>11.5</v>
-      </c>
-      <c r="G46" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="G50" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>3.9473913043478257</v>
-      </c>
-      <c r="H46" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="H50" s="29">
         <f>INDEX(z2nd,13)+Hght_WinWall2</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J46" s="28">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J50" s="28">
         <f>INDEX(x3rd,7)</f>
-        <v>11.5</v>
-      </c>
-      <c r="K46" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="K50" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>3.9473913043478257</v>
-      </c>
-      <c r="L46" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="L50" s="29">
         <f>INDEX(z3rd,13)+Hght_WinWall2</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+        <v>1.8950000000000002</v>
+      </c>
+      <c r="N50" s="24">
+        <v>0</v>
+      </c>
+      <c r="O50" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P50" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="28">
+      <c r="B51" s="28">
         <f>INDEX(x1st,6)</f>
-        <v>11.5</v>
-      </c>
-      <c r="C47" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="C51" s="29">
         <f>INDEX(y1st,6)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D51" s="29">
         <f>INDEX(z1st,14)+Hght_WinWall2</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F47" s="28">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F51" s="28">
         <f>INDEX(x2nd,6)</f>
-        <v>11.5</v>
-      </c>
-      <c r="G47" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="G51" s="29">
         <f>INDEX(y2nd,6)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="H47" s="29">
+      <c r="H51" s="29">
         <f>INDEX(z2nd,14)+Hght_WinWall2</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J47" s="28">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J51" s="28">
         <f>INDEX(x3rd,6)</f>
-        <v>11.5</v>
-      </c>
-      <c r="K47" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="K51" s="29">
         <f>INDEX(y3rd,6)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="L47" s="29">
+      <c r="L51" s="29">
         <f>INDEX(z3rd,14)+Hght_WinWall2</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+        <v>1.8950000000000002</v>
+      </c>
+      <c r="N51" s="25">
+        <f>+Opt_Roof_Peak_W</f>
+        <v>6.45</v>
+      </c>
+      <c r="O51" s="24">
+        <v>0</v>
+      </c>
+      <c r="P51" s="24">
+        <f>+C32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="30">
+      <c r="B52" s="30">
         <f>INDEX(x1st,3)-0.5</f>
-        <v>11</v>
-      </c>
-      <c r="C48" s="31">
+        <v>12.4</v>
+      </c>
+      <c r="C52" s="31">
         <f>INDEX(y1st,3)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D48" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D52" s="31">
         <f>INDEX(z1st,3)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F48" s="30">
+      <c r="F52" s="30">
         <f>INDEX(x2nd,3)-0.5</f>
-        <v>11</v>
-      </c>
-      <c r="G48" s="31">
+        <v>12.4</v>
+      </c>
+      <c r="G52" s="31">
         <f>INDEX(y2nd,3)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H48" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H52" s="31">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J48" s="30">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J52" s="30">
         <f>INDEX(x3rd,3)-0.5</f>
-        <v>11</v>
-      </c>
-      <c r="K48" s="31">
+        <v>12.4</v>
+      </c>
+      <c r="K52" s="31">
         <f>INDEX(y3rd,3)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L48" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L52" s="31">
         <f>INDEX(z3rd,3)+0.5</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="N52" s="25">
+        <f>+Opt_Roof_Peak_W</f>
+        <v>6.45</v>
+      </c>
+      <c r="O52" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P52" s="24">
+        <f>+C32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="30">
+      <c r="B53" s="30">
         <f>INDEX(x1st,17)-Len_WinWall3</f>
-        <v>7.5500000000000007</v>
-      </c>
-      <c r="C49" s="31">
+        <v>5.95</v>
+      </c>
+      <c r="C53" s="31">
         <f>INDEX(y1st,4)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D49" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D53" s="31">
         <f>INDEX(z1st,4)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F49" s="30">
+      <c r="F53" s="30">
         <f>INDEX(x2nd,17)-Len_WinWall3</f>
-        <v>7.5500000000000007</v>
-      </c>
-      <c r="G49" s="31">
+        <v>5.95</v>
+      </c>
+      <c r="G53" s="31">
         <f>INDEX(y2nd,4)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H49" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H53" s="31">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J49" s="30">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J53" s="30">
         <f>INDEX(x3rd,17)-Len_WinWall3</f>
-        <v>7.5500000000000007</v>
-      </c>
-      <c r="K49" s="31">
+        <v>5.95</v>
+      </c>
+      <c r="K53" s="31">
         <f>INDEX(y3rd,4)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L49" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L53" s="31">
         <f>INDEX(z3rd,4)+0.5</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="30">
+      <c r="B54" s="30">
         <f>INDEX(x1st,18)</f>
-        <v>7.5500000000000007</v>
-      </c>
-      <c r="C50" s="31">
+        <v>5.95</v>
+      </c>
+      <c r="C54" s="31">
         <f>INDEX(y1st,18)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D50" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D54" s="31">
         <f>INDEX(z1st,18)+Hght_WinWall3</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F50" s="30">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F54" s="30">
         <f>INDEX(x2nd,18)</f>
-        <v>7.5500000000000007</v>
-      </c>
-      <c r="G50" s="31">
+        <v>5.95</v>
+      </c>
+      <c r="G54" s="31">
         <f>INDEX(y2nd,18)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H50" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H54" s="31">
         <f>INDEX(z2nd,18)+Hght_WinWall3</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J50" s="30">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J54" s="30">
         <f>INDEX(x3rd,18)</f>
-        <v>7.5500000000000007</v>
-      </c>
-      <c r="K50" s="31">
+        <v>5.95</v>
+      </c>
+      <c r="K54" s="31">
         <f>INDEX(y3rd,18)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L50" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L54" s="31">
         <f>INDEX(z3rd,18)+Hght_WinWall3</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+        <v>1.8950000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="30">
+      <c r="B55" s="30">
         <f>INDEX(x1st,17)</f>
-        <v>11</v>
-      </c>
-      <c r="C51" s="31">
+        <v>12.4</v>
+      </c>
+      <c r="C55" s="31">
         <f>INDEX(y1st,19)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="D51" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="D55" s="31">
         <f>INDEX(z1st,19)</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F51" s="30">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F55" s="30">
         <f>INDEX(x2nd,17)</f>
-        <v>11</v>
-      </c>
-      <c r="G51" s="31">
+        <v>12.4</v>
+      </c>
+      <c r="G55" s="31">
         <f>INDEX(y2nd,19)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="H51" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H55" s="31">
         <f>INDEX(z2nd,19)</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J51" s="30">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J55" s="30">
         <f>INDEX(x3rd,17)</f>
-        <v>11</v>
-      </c>
-      <c r="K51" s="31">
+        <v>12.4</v>
+      </c>
+      <c r="K55" s="31">
         <f>INDEX(y3rd,19)</f>
-        <v>11.491304347826087</v>
-      </c>
-      <c r="L51" s="31">
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="L55" s="31">
         <f>INDEX(z3rd,19)</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+        <v>1.8950000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="32">
+      <c r="B56" s="32">
         <f>INDEX(x1st,4)</f>
         <v>0</v>
       </c>
-      <c r="C52" s="32">
+      <c r="C56" s="32">
         <f>INDEX(y1st,4)-0.5</f>
-        <v>10.991304347826087</v>
-      </c>
-      <c r="D52" s="32">
+        <v>8.1344413705656891</v>
+      </c>
+      <c r="D56" s="32">
         <f>INDEX(z1st,4)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F52" s="32">
+      <c r="F56" s="32">
         <f>INDEX(x2nd,4)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="32">
+      <c r="G56" s="32">
         <f>INDEX(y2nd,4)-0.5</f>
-        <v>10.991304347826087</v>
-      </c>
-      <c r="H52" s="32">
+        <v>8.1344413705656891</v>
+      </c>
+      <c r="H56" s="32">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J52" s="32">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J56" s="32">
         <f>INDEX(x3rd,4)</f>
         <v>0</v>
       </c>
-      <c r="K52" s="32">
+      <c r="K56" s="32">
         <f>INDEX(y3rd,4)-0.5</f>
-        <v>10.991304347826087</v>
-      </c>
-      <c r="L52" s="32">
+        <v>8.1344413705656891</v>
+      </c>
+      <c r="L56" s="32">
         <f>INDEX(z3rd,4)+0.5</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="32">
+      <c r="B57" s="32">
         <f>INDEX(x1st,1)</f>
         <v>0</v>
       </c>
-      <c r="C53" s="32">
+      <c r="C57" s="32">
         <f>INDEX(y1st,21)-Len_WinWall4</f>
-        <v>7.5439130434782617</v>
-      </c>
-      <c r="D53" s="32">
+        <v>7.27099723350912</v>
+      </c>
+      <c r="D57" s="32">
         <f>INDEX(z1st,1)+0.5</f>
         <v>2.9384000000000001</v>
       </c>
-      <c r="F53" s="32">
+      <c r="F57" s="32">
         <f>INDEX(x2nd,1)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="32">
+      <c r="G57" s="32">
         <f>INDEX(y2nd,21)-Len_WinWall4</f>
-        <v>7.5439130434782617</v>
-      </c>
-      <c r="H53" s="32">
+        <v>7.27099723350912</v>
+      </c>
+      <c r="H57" s="32">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.9863999999999997</v>
-      </c>
-      <c r="J53" s="32">
+        <v>5.7284000000000006</v>
+      </c>
+      <c r="J57" s="32">
         <f>INDEX(x3rd,1)</f>
         <v>0</v>
       </c>
-      <c r="K53" s="32">
+      <c r="K57" s="32">
         <f>INDEX(y3rd,21)-Len_WinWall4</f>
-        <v>7.5439130434782617</v>
-      </c>
-      <c r="L53" s="32">
+        <v>7.27099723350912</v>
+      </c>
+      <c r="L57" s="32">
         <f>INDEX(z3rd,1)+0.5</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B54" s="32">
+      <c r="B58" s="32">
         <f>INDEX(x1st,5)</f>
         <v>0</v>
       </c>
-      <c r="C54" s="32">
+      <c r="C58" s="32">
         <f>INDEX(y1st,22)</f>
-        <v>7.5439130434782617</v>
-      </c>
-      <c r="D54" s="32">
+        <v>7.27099723350912</v>
+      </c>
+      <c r="D58" s="32">
         <f>INDEX(z1st,22)+Hght_WinWall4</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F54" s="32">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F58" s="32">
         <f>INDEX(x2nd,5)</f>
         <v>0</v>
       </c>
-      <c r="G54" s="32">
+      <c r="G58" s="32">
         <f>INDEX(y2nd,22)</f>
-        <v>7.5439130434782617</v>
-      </c>
-      <c r="H54" s="32">
+        <v>7.27099723350912</v>
+      </c>
+      <c r="H58" s="32">
         <f>INDEX(z2nd,22)+Hght_WinWall4</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J54" s="32">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J58" s="32">
         <f>INDEX(x3rd,5)</f>
         <v>0</v>
       </c>
-      <c r="K54" s="32">
+      <c r="K58" s="32">
         <f>INDEX(y3rd,22)</f>
-        <v>7.5439130434782617</v>
-      </c>
-      <c r="L54" s="32">
+        <v>7.27099723350912</v>
+      </c>
+      <c r="L58" s="32">
         <f>INDEX(z3rd,22)+Hght_WinWall4</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+        <v>1.8950000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="32">
+      <c r="B59" s="32">
         <f>INDEX(x1st,8)</f>
         <v>0</v>
       </c>
-      <c r="C55" s="32">
+      <c r="C59" s="32">
         <f>INDEX(y1st,21)</f>
-        <v>10.991304347826087</v>
-      </c>
-      <c r="D55" s="32">
+        <v>8.1344413705656891</v>
+      </c>
+      <c r="D59" s="32">
         <f>INDEX(z1st,23)</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="F55" s="32">
+        <v>4.3334000000000001</v>
+      </c>
+      <c r="F59" s="32">
         <f>INDEX(x2nd,8)</f>
         <v>0</v>
       </c>
-      <c r="G55" s="32">
+      <c r="G59" s="32">
         <f>INDEX(y2nd,21)</f>
-        <v>10.991304347826087</v>
-      </c>
-      <c r="H55" s="32">
+        <v>8.1344413705656891</v>
+      </c>
+      <c r="H59" s="32">
         <f>INDEX(z2nd,23)</f>
-        <v>7.5103999999999997</v>
-      </c>
-      <c r="J55" s="32">
+        <v>7.1234000000000011</v>
+      </c>
+      <c r="J59" s="32">
         <f>INDEX(x3rd,8)</f>
         <v>0</v>
       </c>
-      <c r="K55" s="32">
+      <c r="K59" s="32">
         <f>INDEX(y3rd,21)</f>
-        <v>10.991304347826087</v>
-      </c>
-      <c r="L55" s="32">
+        <v>8.1344413705656891</v>
+      </c>
+      <c r="L59" s="32">
         <f>INDEX(z3rd,23)</f>
-        <v>2.024</v>
+        <v>1.8950000000000002</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="N45:P45"/>
   </mergeCells>
-  <conditionalFormatting sqref="J30:L55">
+  <conditionalFormatting sqref="J34:L59">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$C$6&lt;3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Geometry options'!$B$3:$B$30</xm:f>
@@ -4114,15 +4407,15 @@
       </c>
       <c r="E7" s="55">
         <f>+main_area+second_area+third_area</f>
-        <v>214.4996730434782</v>
+        <v>193.98154031771418</v>
       </c>
       <c r="F7" s="55">
         <f>+E7*10.7639</f>
-        <v>2308.8530306726948</v>
+        <v>2087.9979018258437</v>
       </c>
       <c r="G7" s="81">
         <f>+D7*F7</f>
-        <v>22031.588697130112</v>
+        <v>19924.139978755939</v>
       </c>
       <c r="H7" t="s">
         <v>143</v>
@@ -4171,15 +4464,15 @@
       </c>
       <c r="E10" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>214.4996730434782</v>
+        <v>193.98154031771418</v>
       </c>
       <c r="F10" s="55">
         <f>+E10*10.7639</f>
-        <v>2308.8530306726948</v>
+        <v>2087.9979018258437</v>
       </c>
       <c r="G10" s="81">
         <f>+D10*F10</f>
-        <v>24145.471916323782</v>
+        <v>21835.818057760935</v>
       </c>
       <c r="H10" t="s">
         <v>144</v>
@@ -4228,15 +4521,15 @@
       </c>
       <c r="E13" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>214.4996730434782</v>
+        <v>193.98154031771418</v>
       </c>
       <c r="F13" s="55">
         <f>+E13*10.7639</f>
-        <v>2308.8530306726948</v>
+        <v>2087.9979018258437</v>
       </c>
       <c r="G13" s="81">
         <f>+D13*F13</f>
-        <v>21957.192321697326</v>
+        <v>19856.860046363774</v>
       </c>
       <c r="H13" t="s">
         <v>172</v>
@@ -4285,15 +4578,15 @@
       </c>
       <c r="E16" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>214.4996730434782</v>
+        <v>193.98154031771418</v>
       </c>
       <c r="F16" s="55">
         <f>+E16*10.7639</f>
-        <v>2308.8530306726948</v>
+        <v>2087.9979018258437</v>
       </c>
       <c r="G16" s="81">
         <f t="shared" ref="G16:G17" si="0">+D16*F16</f>
-        <v>34632.79546009042</v>
+        <v>31319.968527387653</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -4309,15 +4602,15 @@
       </c>
       <c r="E17" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>214.4996730434782</v>
+        <v>193.98154031771418</v>
       </c>
       <c r="F17" s="55">
         <f>+E17*10.7639</f>
-        <v>2308.8530306726948</v>
+        <v>2087.9979018258437</v>
       </c>
       <c r="G17" s="81">
         <f t="shared" si="0"/>
-        <v>37068.635407450114</v>
+        <v>33522.806313813919</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4370,15 +4663,15 @@
       </c>
       <c r="E21" s="55">
         <f>found_wall_area</f>
-        <v>112.12399304347827</v>
+        <v>105.01916367597477</v>
       </c>
       <c r="F21" s="55">
         <f>+E21*10.7639</f>
-        <v>1206.8914487206957</v>
+        <v>1130.4157758918248</v>
       </c>
       <c r="G21" s="68">
         <f>+F21*D21</f>
-        <v>5262.0467164222327</v>
+        <v>4928.6127828883555</v>
       </c>
       <c r="H21" t="s">
         <v>173</v>
@@ -4425,15 +4718,15 @@
       </c>
       <c r="E24" s="55">
         <f>found_wall_area</f>
-        <v>112.12399304347827</v>
+        <v>105.01916367597477</v>
       </c>
       <c r="F24" s="55">
         <f>+E24*10.7639</f>
-        <v>1206.8914487206957</v>
+        <v>1130.4157758918248</v>
       </c>
       <c r="G24" s="68">
         <f>+F24*D24</f>
-        <v>10741.333893614195</v>
+        <v>10060.700405437243</v>
       </c>
       <c r="H24" t="s">
         <v>174</v>
@@ -4461,15 +4754,15 @@
       </c>
       <c r="E26" s="55">
         <f>+Opt_Area</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="F26" s="55">
         <f>+E26*10.7639</f>
-        <v>1422.4493849999999</v>
+        <v>1198.929398745353</v>
       </c>
       <c r="G26" s="68">
         <f>+F26*D26</f>
-        <v>1308.6534342</v>
+        <v>1103.0150468457248</v>
       </c>
       <c r="H26" t="s">
         <v>170</v>
@@ -4488,15 +4781,15 @@
       </c>
       <c r="E27" s="55">
         <f>+Opt_Area</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="F27" s="55">
         <f>+E27*10.7639</f>
-        <v>1422.4493849999999</v>
+        <v>1198.929398745353</v>
       </c>
       <c r="G27" s="68">
         <f>+F27*D27</f>
-        <v>1422.4493849999999</v>
+        <v>1198.929398745353</v>
       </c>
       <c r="H27" t="s">
         <v>171</v>
@@ -4623,15 +4916,15 @@
       </c>
       <c r="E37" s="47">
         <f>total_window_area</f>
-        <v>37.852883478260864</v>
+        <v>31.268716418402928</v>
       </c>
       <c r="F37" s="55">
         <f t="shared" ref="F37:F40" si="1">+E37*10.7639</f>
-        <v>407.44465247165209</v>
+        <v>336.57333665604727</v>
       </c>
       <c r="G37" s="68">
         <f>+D37*F37</f>
-        <v>28764.265476107936</v>
+        <v>23760.981397166746</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -4647,15 +4940,15 @@
       </c>
       <c r="E38" s="89">
         <f>total_window_area</f>
-        <v>37.852883478260864</v>
+        <v>31.268716418402928</v>
       </c>
       <c r="F38" s="55">
         <f t="shared" si="1"/>
-        <v>407.44465247165209</v>
+        <v>336.57333665604727</v>
       </c>
       <c r="G38" s="68">
         <f t="shared" ref="G38:G40" si="2">+D38*F38</f>
-        <v>28764.265476107936</v>
+        <v>23760.981397166746</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -4671,15 +4964,15 @@
       </c>
       <c r="E39" s="89">
         <f>total_window_area</f>
-        <v>37.852883478260864</v>
+        <v>31.268716418402928</v>
       </c>
       <c r="F39" s="55">
         <f t="shared" si="1"/>
-        <v>407.44465247165209</v>
+        <v>336.57333665604727</v>
       </c>
       <c r="G39" s="68">
         <f t="shared" si="2"/>
-        <v>32126.523679132039</v>
+        <v>26538.405165588203</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -4695,15 +4988,15 @@
       </c>
       <c r="E40" s="89">
         <f>total_window_area</f>
-        <v>37.852883478260864</v>
+        <v>31.268716418402928</v>
       </c>
       <c r="F40" s="55">
         <f t="shared" si="1"/>
-        <v>407.44465247165209</v>
+        <v>336.57333665604727</v>
       </c>
       <c r="G40" s="68">
         <f t="shared" si="2"/>
-        <v>32126.523679132039</v>
+        <v>26538.405165588203</v>
       </c>
     </row>
   </sheetData>
@@ -4787,11 +5080,11 @@
       <c r="H3" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="93" t="s">
+      <c r="I3" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
Addition of Mattamy Ottawa archetype
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-2st-garage/model_geometry_with_garage.xlsx
+++ b/OptFramework/GenericHome-2st-garage/model_geometry_with_garage.xlsx
@@ -182,6 +182,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="I10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jeffblake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Right windows actually 0 but need a non-zero value here!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jeffblake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+9 7/8" : 12 roof slope</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jeffblake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ACH range for base is 2.2 to 2.4 ACH from conversation with Shane.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -222,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="194">
   <si>
     <t>m²</t>
   </si>
@@ -692,9 +764,6 @@
     <t>GenOpt Tag</t>
   </si>
   <si>
-    <t>Window to Wall Ratio</t>
-  </si>
-  <si>
     <t>Front</t>
   </si>
   <si>
@@ -795,6 +864,18 @@
   </si>
   <si>
     <t>NZEH-Arch</t>
+  </si>
+  <si>
+    <t>Mattamy_Ott</t>
+  </si>
+  <si>
+    <t>Archetype for Mattamy Homes - Ottawa - November 2014</t>
+  </si>
+  <si>
+    <t>Window to Wall Ratio (%)</t>
+  </si>
+  <si>
+    <t>Number of storeys (a.g.)</t>
   </si>
 </sst>
 </file>
@@ -806,7 +887,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -920,6 +1001,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -990,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1180,6 +1274,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1717,10 +1826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U9"/>
+  <dimension ref="B1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,26 +1843,28 @@
     <col min="7" max="7" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="10.42578125" style="47" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11.28515625" style="47" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="20" width="12.28515625" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="94" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="94" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="94" customWidth="1"/>
+    <col min="17" max="17" width="11" style="94" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" style="94" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="98" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" style="94" customWidth="1"/>
+    <col min="21" max="21" width="75.140625" customWidth="1"/>
     <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H1" s="94" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="S1" s="95" t="s">
-        <v>182</v>
-      </c>
-      <c r="T1" s="95"/>
+      <c r="H1" s="99" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="S1" s="100" t="s">
+        <v>181</v>
+      </c>
+      <c r="T1" s="100"/>
     </row>
     <row r="2" spans="2:21" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1763,7 +1874,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="71" t="s">
-        <v>69</v>
+        <v>193</v>
       </c>
       <c r="E2" s="72" t="s">
         <v>85</v>
@@ -1775,43 +1886,43 @@
         <v>151</v>
       </c>
       <c r="H2" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="K2" s="73" t="s">
         <v>159</v>
-      </c>
-      <c r="J2" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="K2" s="73" t="s">
-        <v>160</v>
       </c>
       <c r="L2" s="70" t="s">
         <v>148</v>
       </c>
       <c r="M2" s="70" t="s">
-        <v>169</v>
-      </c>
-      <c r="N2" s="73" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="73" t="s">
+      <c r="O2" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="P2" s="73" t="s">
+      <c r="P2" s="95" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="73" t="s">
+      <c r="Q2" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="73" t="s">
+      <c r="R2" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="S2" s="73" t="s">
+      <c r="S2" s="95" t="s">
+        <v>185</v>
+      </c>
+      <c r="T2" s="95" t="s">
         <v>186</v>
-      </c>
-      <c r="T2" s="73" t="s">
-        <v>187</v>
       </c>
       <c r="U2" s="70" t="s">
         <v>147</v>
@@ -1835,7 +1946,7 @@
         <v>11.5</v>
       </c>
       <c r="G3" s="66">
-        <f t="shared" ref="G3:G9" si="0">+E3/F3</f>
+        <f t="shared" ref="G3:G10" si="0">+E3/F3</f>
         <v>11.491304347826087</v>
       </c>
       <c r="H3" s="47">
@@ -1874,10 +1985,10 @@
       <c r="R3" s="85">
         <v>2</v>
       </c>
-      <c r="S3" s="85"/>
+      <c r="S3" s="96"/>
       <c r="T3" s="85"/>
       <c r="U3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
@@ -1891,7 +2002,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="66">
-        <f>+C4/D4</f>
+        <f t="shared" ref="E4:E9" si="1">+C4/D4</f>
         <v>83.333333333333329</v>
       </c>
       <c r="F4" s="66">
@@ -1934,7 +2045,7 @@
       <c r="R4" s="85">
         <v>2</v>
       </c>
-      <c r="S4" s="85"/>
+      <c r="S4" s="96"/>
       <c r="T4" s="85"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
@@ -1948,7 +2059,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="47">
-        <f>+C5/D5</f>
+        <f t="shared" si="1"/>
         <v>95.100000000000009</v>
       </c>
       <c r="F5" s="47">
@@ -1992,12 +2103,12 @@
       <c r="R5" s="85">
         <v>2</v>
       </c>
-      <c r="S5" s="85"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="85"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="86">
         <f>2396.99/10.76</f>
@@ -2007,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="86">
-        <f>+C6/D6</f>
+        <f t="shared" si="1"/>
         <v>111.38429368029739</v>
       </c>
       <c r="F6" s="82">
@@ -2053,15 +2164,15 @@
       <c r="R6" s="88">
         <v>1.9</v>
       </c>
-      <c r="S6" s="88"/>
+      <c r="S6" s="97"/>
       <c r="T6" s="88"/>
       <c r="U6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C7" s="47">
         <v>167.5</v>
@@ -2070,7 +2181,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="86">
-        <f>+C7/D7</f>
+        <f t="shared" si="1"/>
         <v>55.833333333333336</v>
       </c>
       <c r="F7" s="47">
@@ -2114,7 +2225,7 @@
       <c r="R7" s="88">
         <v>1.9</v>
       </c>
-      <c r="S7" s="88">
+      <c r="S7" s="97">
         <v>3.3018999999999998</v>
       </c>
       <c r="T7" s="88">
@@ -2123,7 +2234,7 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" s="92">
         <v>125</v>
@@ -2132,7 +2243,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="86">
-        <f>+C8/D8</f>
+        <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
       <c r="F8" s="92">
@@ -2176,7 +2287,7 @@
       <c r="R8" s="88">
         <v>1.9</v>
       </c>
-      <c r="S8" s="88">
+      <c r="S8" s="97">
         <v>3.3018999999999998</v>
       </c>
       <c r="T8" s="88">
@@ -2185,7 +2296,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="86">
         <f>2396.99/10.76</f>
@@ -2195,7 +2306,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="86">
-        <f>+C9/D9</f>
+        <f t="shared" si="1"/>
         <v>111.38429368029739</v>
       </c>
       <c r="F9" s="47">
@@ -2238,10 +2349,73 @@
       <c r="R9" s="88">
         <v>1.9</v>
       </c>
-      <c r="S9" s="88"/>
+      <c r="S9" s="97"/>
       <c r="T9" s="88"/>
       <c r="U9" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="94">
+        <v>178.8</v>
+      </c>
+      <c r="D10" s="94">
+        <v>2</v>
+      </c>
+      <c r="E10" s="94">
+        <v>89.4</v>
+      </c>
+      <c r="F10" s="94">
+        <v>7.24</v>
+      </c>
+      <c r="G10" s="68">
+        <f t="shared" si="0"/>
+        <v>12.348066298342541</v>
+      </c>
+      <c r="H10" s="94">
+        <v>19</v>
+      </c>
+      <c r="I10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="94">
+        <v>25</v>
+      </c>
+      <c r="K10" s="94">
+        <v>8</v>
+      </c>
+      <c r="L10" s="94">
+        <v>0.82</v>
+      </c>
+      <c r="M10" s="94">
+        <v>2.4</v>
+      </c>
+      <c r="N10" s="94">
+        <v>2.72</v>
+      </c>
+      <c r="O10" s="94">
+        <v>2.46</v>
+      </c>
+      <c r="P10" s="94">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="94">
+        <v>2.59</v>
+      </c>
+      <c r="R10" s="94">
+        <v>2.13</v>
+      </c>
+      <c r="S10" s="98">
+        <v>3</v>
+      </c>
+      <c r="T10" s="94">
+        <v>6.05</v>
+      </c>
+      <c r="U10" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2250,7 +2424,7 @@
     <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2259,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2488,7 @@
       <c r="D4" s="1"/>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
-      <c r="H4" s="98" t="s">
+      <c r="H4" s="103" t="s">
         <v>89</v>
       </c>
       <c r="I4" s="58" t="s">
@@ -2334,7 +2508,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="64">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,2,FALSE)</f>
-        <v>222.76858736059478</v>
+        <v>178.8</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -2345,12 +2519,12 @@
       <c r="G5" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="97" t="s">
+      <c r="H5" s="104"/>
+      <c r="I5" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2370,11 +2544,11 @@
       </c>
       <c r="I6" s="33">
         <f>+(INDEX(x1st,2)-INDEX(x1st,1))*(INDEX(z1st,7)-INDEX(z1st,2))</f>
-        <v>35.991000000000007</v>
+        <v>19.692800000000005</v>
       </c>
       <c r="J6" s="33">
         <f>+(INDEX(x2nd,2)-INDEX(x2nd,1))*(INDEX(z2nd,7)-INDEX(z2nd,2))</f>
-        <v>31.475999999999996</v>
+        <v>17.810400000000001</v>
       </c>
       <c r="K6" s="33">
         <f>+(INDEX(x3rd,2)-INDEX(x3rd,1))*(INDEX(z3rd,7)-INDEX(z3rd,2))</f>
@@ -2393,7 +2567,7 @@
       </c>
       <c r="C7" s="11">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,4,FALSE)</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>0</v>
@@ -2406,11 +2580,11 @@
       </c>
       <c r="I7" s="33">
         <f>+(INDEX(y1st,3)-INDEX(y1st,2))*(INDEX(z1st,7)-(INDEX(z1st,3)))</f>
-        <v>24.090091423878278</v>
+        <v>33.586740331491718</v>
       </c>
       <c r="J7" s="33">
         <f>+(INDEX(y2nd,3)-INDEX(y2nd,2))*(INDEX(z2nd,7)-(INDEX(z2nd,3)))</f>
-        <v>21.068036944180278</v>
+        <v>30.37624309392265</v>
       </c>
       <c r="K7" s="33">
         <f>+(INDEX(y3rd,3)-INDEX(y3rd,2))*(INDEX(z3rd,7)-(INDEX(z3rd,3)))</f>
@@ -2429,7 +2603,7 @@
       </c>
       <c r="C8" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,5,FALSE)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="D8" s="39" t="s">
         <v>1</v>
@@ -2442,11 +2616,11 @@
       </c>
       <c r="I8" s="33">
         <f>(INDEX(x1st,3)-INDEX(x1st,4))*(INDEX(z1st,7)-INDEX(z1st,4))</f>
-        <v>35.991000000000007</v>
+        <v>19.692800000000005</v>
       </c>
       <c r="J8" s="33">
         <f>(INDEX(x2nd,3)-INDEX(x2nd,4))*(INDEX(z2nd,7)-INDEX(z2nd,4))</f>
-        <v>31.475999999999996</v>
+        <v>17.810400000000001</v>
       </c>
       <c r="K8" s="33">
         <f>(INDEX(x3rd,3)-INDEX(x3rd,4))*(INDEX(z3rd,7)-INDEX(z3rd,4))</f>
@@ -2465,7 +2639,7 @@
       </c>
       <c r="C9" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,6,FALSE)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>1</v>
@@ -2479,11 +2653,11 @@
       </c>
       <c r="I9" s="33">
         <f>(INDEX(y1st,4)-INDEX(y1st,1))*(INDEX(z1st,8)-INDEX(z1st,4))</f>
-        <v>24.090091423878278</v>
+        <v>33.586740331491718</v>
       </c>
       <c r="J9" s="33">
         <f>(INDEX(y2nd,4)-INDEX(y2nd,1))*(INDEX(z2nd,8)-INDEX(z2nd,4))</f>
-        <v>21.068036944180278</v>
+        <v>30.37624309392265</v>
       </c>
       <c r="K9" s="33">
         <f>(INDEX(y3rd,4)-INDEX(y3rd,1))*(INDEX(z3rd,8)-INDEX(z3rd,4))</f>
@@ -2500,7 +2674,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,13,FALSE)</f>
-        <v>2.79</v>
+        <v>2.72</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -2513,15 +2687,15 @@
       </c>
       <c r="I10" s="33">
         <f>INDEX(x1st,6)*INDEX(y1st,7)</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="J10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="K10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="L10" t="s">
         <v>0</v>
@@ -2534,7 +2708,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,14,FALSE)</f>
-        <v>2.44</v>
+        <v>2.46</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
@@ -2547,15 +2721,15 @@
       </c>
       <c r="I11" s="33">
         <f>INDEX(x1st,3)*INDEX(y1st,4)</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="J11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="K11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="L11" t="s">
         <v>0</v>
@@ -2587,15 +2761,15 @@
       </c>
       <c r="H12" s="43">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,7,FALSE)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I12" s="15">
         <f>AreaWall1*AreaWinWall1Ratio/100</f>
-        <v>6.4783800000000005</v>
+        <v>3.741632000000001</v>
       </c>
       <c r="J12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>5.6656799999999983</v>
+        <v>3.3839760000000001</v>
       </c>
       <c r="K12" s="15">
         <f>+IF(NumStoreys=3,AreaWall1_2nd*AreaWinWall1Ratio/100,0)</f>
@@ -2606,15 +2780,15 @@
       </c>
       <c r="M12" s="27">
         <f>AreaWinWall1/Hght_WinWall1</f>
-        <v>4.6439999999999992</v>
+        <v>2.7511999999999999</v>
       </c>
       <c r="N12" s="26">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.3600000000000003</v>
       </c>
       <c r="O12">
         <f>+Len_WinWall1*Hght_WinWall1</f>
-        <v>6.4783800000000005</v>
+        <v>3.7416320000000005</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2624,7 +2798,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,16,FALSE)</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -2637,15 +2811,15 @@
       </c>
       <c r="H13" s="44">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,8,FALSE)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="17">
         <f>AreaWall2*AreaWinWall2Ratio/100</f>
-        <v>0</v>
+        <v>0.16793370165745858</v>
       </c>
       <c r="J13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>0</v>
+        <v>0.15188121546961325</v>
       </c>
       <c r="K13" s="17">
         <f>+IF(NumStoreys=3,AreaWall2_2nd*AreaWinWall2Ratio/100,0)</f>
@@ -2656,15 +2830,15 @@
       </c>
       <c r="M13" s="28">
         <f>AreaWinWall2/Hght_WinWall2</f>
-        <v>0</v>
+        <v>0.1234806629834254</v>
       </c>
       <c r="N13" s="29">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.3600000000000003</v>
       </c>
       <c r="O13">
         <f>+Len_WinWall2*Hght_WinWall2</f>
-        <v>0</v>
+        <v>0.16793370165745858</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2674,7 +2848,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,17,FALSE)</f>
-        <v>1.9</v>
+        <v>2.13</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -2691,11 +2865,11 @@
       </c>
       <c r="I14" s="18">
         <f>AreaWall3*AreaWinWall3Ratio/100</f>
-        <v>8.9977500000000017</v>
+        <v>4.9232000000000014</v>
       </c>
       <c r="J14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>7.8689999999999989</v>
+        <v>4.4526000000000003</v>
       </c>
       <c r="K14" s="18">
         <f>+IF(NumStoreys=3,AreaWall3_2nd*AreaWinWall3Ratio/100,0)</f>
@@ -2706,15 +2880,15 @@
       </c>
       <c r="M14" s="30">
         <f>AreaWinWall3/Hght_WinWall3</f>
-        <v>6.45</v>
+        <v>3.62</v>
       </c>
       <c r="N14" s="31">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.3600000000000003</v>
       </c>
       <c r="O14">
         <f>+Len_WinWall3*Hght_WinWall3</f>
-        <v>8.9977500000000017</v>
+        <v>4.9232000000000014</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2724,7 +2898,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="39">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>49</v>
@@ -2737,11 +2911,11 @@
       </c>
       <c r="I15" s="20">
         <f>AreaWall4*AreaWinWall4Ratio/100</f>
-        <v>1.204504571193914</v>
+        <v>1.6793370165745858</v>
       </c>
       <c r="J15" s="20">
         <f>AreaWall4_2nd*AreaWinWall4Ratio/100</f>
-        <v>1.0534018472090139</v>
+        <v>1.5188121546961324</v>
       </c>
       <c r="K15" s="20">
         <f>+IF(NumStoreys=3,AreaWall4_2nd*AreaWinWall4Ratio/100,0)</f>
@@ -2752,15 +2926,15 @@
       </c>
       <c r="M15" s="36">
         <f>AreaWinWall4/Hght_WinWall4</f>
-        <v>0.86344413705656897</v>
+        <v>1.2348066298342539</v>
       </c>
       <c r="N15" s="32">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.3600000000000003</v>
       </c>
       <c r="O15">
         <f>+Len_WinWall4*Hght_WinWall4</f>
-        <v>1.204504571193914</v>
+        <v>1.6793370165745858</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2770,7 +2944,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="74">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,11,FALSE)</f>
-        <v>0.66700000000000004</v>
+        <v>0.82</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2785,11 +2959,11 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" s="35">
         <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Roof_Peak_W*Roof_Slope1)</f>
-        <v>11.970549999999999</v>
+        <v>10.7384</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -2811,20 +2985,20 @@
       </c>
       <c r="C18" s="11">
         <f>Opt_Width/2</f>
-        <v>6.45</v>
+        <v>3.62</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C19" s="11">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,18,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -2833,11 +3007,11 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C20" s="11">
         <f>VLOOKUP($B$2,'Geometry options'!B4:U39,19,FALSE)</f>
-        <v>0</v>
+        <v>6.05</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
@@ -2846,11 +3020,11 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C21" s="11">
         <f>+C19*C20</f>
-        <v>0</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>0</v>
@@ -2876,7 +3050,7 @@
       </c>
       <c r="I23" s="42">
         <f>SUM(I6:I9)-SUM(I12:I15)</f>
-        <v>103.48154827656265</v>
+        <v>96.04697794475139</v>
       </c>
       <c r="J23" t="s">
         <v>0</v>
@@ -2888,7 +3062,7 @@
       </c>
       <c r="C24" s="15">
         <f>INDEX(x1st,10)</f>
-        <v>5.1439999999999992</v>
+        <v>3.2511999999999999</v>
       </c>
       <c r="D24" s="1"/>
       <c r="F24" t="s">
@@ -2896,7 +3070,7 @@
       </c>
       <c r="I24" s="90">
         <f>+SUM(J6:J9)-SUM(J12:J15)</f>
-        <v>90.499992041151543</v>
+        <v>86.866016817679565</v>
       </c>
       <c r="J24" t="s">
         <v>0</v>
@@ -2931,14 +3105,14 @@
       </c>
       <c r="C26" s="17">
         <f>INDEX(y1st,14)</f>
-        <v>0.5</v>
+        <v>0.62348066298342542</v>
       </c>
       <c r="F26" t="s">
         <v>136</v>
       </c>
       <c r="I26">
         <f>2*(Opt_Width*Opt_Bsm_Height)+2*(Opt_Length*Opt_Bsm_Height)</f>
-        <v>105.01916367597477</v>
+        <v>101.46618342541436</v>
       </c>
       <c r="J26" t="s">
         <v>0</v>
@@ -2951,21 +3125,21 @@
       </c>
       <c r="C27" s="18">
         <f>INDEX(x1st,17)</f>
-        <v>12.4</v>
+        <v>6.74</v>
       </c>
       <c r="F27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I27">
         <f>+AreaWinWall1Ratio/100*SUM(I6:K6)+AreaWinWall2Ratio/100*SUM(I7:K7)+AreaWinWall3Ratio/100*SUM(I8:K8)+AreaWinWall4Ratio/100*SUM(I9:K9)</f>
-        <v>31.268716418402928</v>
+        <v>20.019372088397791</v>
       </c>
       <c r="J27" t="s">
         <v>0</v>
       </c>
       <c r="K27" s="90">
         <f>+SUM(I12:K15)</f>
-        <v>31.268716418402928</v>
+        <v>20.019372088397791</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2975,7 +3149,7 @@
       </c>
       <c r="C28" s="18">
         <f>INDEX(x1st,18)</f>
-        <v>5.95</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2984,7 +3158,7 @@
       </c>
       <c r="C29" s="19">
         <f>INDEX(y1st,21)</f>
-        <v>8.1344413705656891</v>
+        <v>11.848066298342541</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -2993,7 +3167,7 @@
       </c>
       <c r="C30" s="20">
         <f>INDEX(y1st,22)</f>
-        <v>7.27099723350912</v>
+        <v>10.613259668508288</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -3001,31 +3175,31 @@
       <c r="C33" s="61"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="96" t="s">
+      <c r="B34" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="96"/>
-      <c r="D34" s="96"/>
-      <c r="F34" s="96" t="s">
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="F34" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="G34" s="96"/>
-      <c r="H34" s="96"/>
-      <c r="J34" s="96" t="s">
+      <c r="G34" s="101"/>
+      <c r="H34" s="101"/>
+      <c r="J34" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="K34" s="96"/>
-      <c r="L34" s="96"/>
-      <c r="N34" s="96" t="s">
+      <c r="K34" s="101"/>
+      <c r="L34" s="101"/>
+      <c r="N34" s="101" t="s">
+        <v>174</v>
+      </c>
+      <c r="O34" s="101"/>
+      <c r="P34" s="101"/>
+      <c r="R34" s="101" t="s">
         <v>175</v>
       </c>
-      <c r="O34" s="96"/>
-      <c r="P34" s="96"/>
-      <c r="R34" s="96" t="s">
-        <v>176</v>
-      </c>
-      <c r="S34" s="96"/>
-      <c r="T34" s="96"/>
+      <c r="S34" s="101"/>
+      <c r="T34" s="101"/>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
@@ -3089,7 +3263,7 @@
       </c>
       <c r="D36" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
@@ -3099,7 +3273,7 @@
       </c>
       <c r="H36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="J36" s="24">
         <v>0</v>
@@ -3119,7 +3293,7 @@
       </c>
       <c r="P36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="R36" s="24">
         <v>0</v>
@@ -3137,29 +3311,29 @@
       </c>
       <c r="B37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C37" s="24">
         <v>0</v>
       </c>
       <c r="D37" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
       <c r="F37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G37" s="24">
         <v>0</v>
       </c>
       <c r="H37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="J37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K37" s="24">
         <v>0</v>
@@ -3170,18 +3344,18 @@
       </c>
       <c r="N37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="O37" s="24">
         <v>0</v>
       </c>
       <c r="P37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="R37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="S37" s="24">
         <v>0</v>
@@ -3196,35 +3370,35 @@
       </c>
       <c r="B38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D38" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
       <c r="F38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="J38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L38" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
@@ -3232,23 +3406,23 @@
       </c>
       <c r="N38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="O38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="P38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="R38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="S38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="T38" s="24">
         <v>0</v>
@@ -3263,29 +3437,29 @@
       </c>
       <c r="C39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D39" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
       </c>
       <c r="G39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="J39" s="24">
         <v>0</v>
       </c>
       <c r="K39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L39" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
@@ -3296,18 +3470,18 @@
       </c>
       <c r="O39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="P39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="R39" s="24">
         <v>0</v>
       </c>
       <c r="S39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="T39" s="24">
         <v>0</v>
@@ -3325,7 +3499,7 @@
       </c>
       <c r="D40" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="F40" s="24">
         <v>0</v>
@@ -3335,7 +3509,7 @@
       </c>
       <c r="H40" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="J40" s="24">
         <v>0</v>
@@ -3349,14 +3523,14 @@
       </c>
       <c r="N40" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.62</v>
       </c>
       <c r="O40" s="24">
         <v>0</v>
       </c>
       <c r="P40" s="24">
         <f>+C17</f>
-        <v>11.970549999999999</v>
+        <v>10.7384</v>
       </c>
       <c r="R40" s="24">
         <v>0</v>
@@ -3366,7 +3540,7 @@
       </c>
       <c r="T40" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -3375,29 +3549,29 @@
       </c>
       <c r="B41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C41" s="24">
         <v>0</v>
       </c>
       <c r="D41" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="F41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G41" s="24">
         <v>0</v>
       </c>
       <c r="H41" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="J41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K41" s="24">
         <v>0</v>
@@ -3408,26 +3582,26 @@
       </c>
       <c r="N41" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.62</v>
       </c>
       <c r="O41" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="P41" s="24">
         <f>+C17</f>
-        <v>11.970549999999999</v>
+        <v>10.7384</v>
       </c>
       <c r="R41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="S41" s="24">
         <v>0</v>
       </c>
       <c r="T41" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -3436,35 +3610,35 @@
       </c>
       <c r="B42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D42" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="F42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H42" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="J42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L42" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
@@ -3474,15 +3648,15 @@
       <c r="O42" s="84"/>
       <c r="R42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="S42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="T42" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -3494,29 +3668,29 @@
       </c>
       <c r="C43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D43" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.3100000000000005</v>
       </c>
       <c r="F43" s="24">
         <v>0</v>
       </c>
       <c r="G43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H43" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="J43" s="24">
         <v>0</v>
       </c>
       <c r="K43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L43" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
@@ -3529,11 +3703,11 @@
       </c>
       <c r="S43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="T43" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -3550,7 +3724,7 @@
       </c>
       <c r="D44" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F44" s="26">
         <f>INDEX(x2nd,1)+0.5</f>
@@ -3562,7 +3736,7 @@
       </c>
       <c r="H44" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J44" s="26">
         <f>INDEX(x3rd,1)+0.5</f>
@@ -3583,7 +3757,7 @@
       </c>
       <c r="B45" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.2511999999999999</v>
       </c>
       <c r="C45" s="26">
         <f>INDEX(y1st,2)</f>
@@ -3591,11 +3765,11 @@
       </c>
       <c r="D45" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F45" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.2511999999999999</v>
       </c>
       <c r="G45" s="26">
         <f>INDEX(y2nd,2)</f>
@@ -3603,11 +3777,11 @@
       </c>
       <c r="H45" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J45" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.2511999999999999</v>
       </c>
       <c r="K45" s="26">
         <f>INDEX(y3rd,2)</f>
@@ -3617,11 +3791,11 @@
         <f>INDEX(z3rd,1)+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="N45" s="96" t="s">
-        <v>181</v>
-      </c>
-      <c r="O45" s="96"/>
-      <c r="P45" s="96"/>
+      <c r="N45" s="101" t="s">
+        <v>180</v>
+      </c>
+      <c r="O45" s="101"/>
+      <c r="P45" s="101"/>
     </row>
     <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
@@ -3629,7 +3803,7 @@
       </c>
       <c r="B46" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.2511999999999999</v>
       </c>
       <c r="C46" s="26">
         <f>INDEX(y1st,5)</f>
@@ -3637,11 +3811,11 @@
       </c>
       <c r="D46" s="26">
         <f>INDEX(z1st,9)+Hght_WinWall1</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F46" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.2511999999999999</v>
       </c>
       <c r="G46" s="26">
         <f>INDEX(y2nd,5)</f>
@@ -3649,11 +3823,11 @@
       </c>
       <c r="H46" s="26">
         <f>INDEX(z2nd,9)+Hght_WinWall1</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J46" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.2511999999999999</v>
       </c>
       <c r="K46" s="26">
         <f>INDEX(y3rd,5)</f>
@@ -3661,7 +3835,7 @@
       </c>
       <c r="L46" s="26">
         <f>INDEX(z3rd,9)+Hght_WinWall1</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
       <c r="N46" s="91" t="s">
         <v>2</v>
@@ -3687,7 +3861,7 @@
       </c>
       <c r="D47" s="26">
         <f>INDEX(z1st,10)+Hght_WinWall1</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F47" s="26">
         <f>INDEX(x2nd,9)</f>
@@ -3699,7 +3873,7 @@
       </c>
       <c r="H47" s="26">
         <f>INDEX(z2nd,10)+Hght_WinWall1</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J47" s="26">
         <f>INDEX(x3rd,9)</f>
@@ -3711,7 +3885,7 @@
       </c>
       <c r="L47" s="26">
         <f>INDEX(z3rd,10)+Hght_WinWall1</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
       <c r="N47" s="24">
         <v>0</v>
@@ -3721,7 +3895,7 @@
       </c>
       <c r="P47" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -3730,7 +3904,7 @@
       </c>
       <c r="B48" s="28">
         <f>INDEX(x1st,2)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C48" s="29">
         <f>INDEX(y1st,2)+0.5</f>
@@ -3738,11 +3912,11 @@
       </c>
       <c r="D48" s="29">
         <f>INDEX(z1st,2)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F48" s="28">
         <f>INDEX(x2nd,2)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G48" s="29">
         <f>INDEX(y2nd,2)+0.5</f>
@@ -3750,11 +3924,11 @@
       </c>
       <c r="H48" s="29">
         <f>INDEX(z2nd,2)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J48" s="28">
         <f>INDEX(x3rd,2)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K48" s="29">
         <f>INDEX(y3rd,2)+0.5</f>
@@ -3766,14 +3940,14 @@
       </c>
       <c r="N48" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="O48" s="24">
         <v>0</v>
       </c>
       <c r="P48" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3782,35 +3956,35 @@
       </c>
       <c r="B49" s="28">
         <f>INDEX(x1st,3)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C49" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>0.62348066298342542</v>
       </c>
       <c r="D49" s="29">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F49" s="28">
         <f>INDEX(x2nd,3)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G49" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>0.62348066298342542</v>
       </c>
       <c r="H49" s="29">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J49" s="28">
         <f>INDEX(x3rd,3)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K49" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>0.62348066298342542</v>
       </c>
       <c r="L49" s="29">
         <f>INDEX(z3rd,3)+0.5</f>
@@ -3818,15 +3992,15 @@
       </c>
       <c r="N49" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="O49" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="P49" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3835,50 +4009,50 @@
       </c>
       <c r="B50" s="28">
         <f>INDEX(x1st,7)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C50" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>0.62348066298342542</v>
       </c>
       <c r="D50" s="29">
         <f>INDEX(z1st,13)+Hght_WinWall2</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F50" s="28">
         <f>INDEX(x2nd,7)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G50" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>0.62348066298342542</v>
       </c>
       <c r="H50" s="29">
         <f>INDEX(z2nd,13)+Hght_WinWall2</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J50" s="28">
         <f>INDEX(x3rd,7)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K50" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>0.62348066298342542</v>
       </c>
       <c r="L50" s="29">
         <f>INDEX(z3rd,13)+Hght_WinWall2</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
       <c r="N50" s="24">
         <v>0</v>
       </c>
       <c r="O50" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="P50" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.7700000000000005</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3887,7 +4061,7 @@
       </c>
       <c r="B51" s="28">
         <f>INDEX(x1st,6)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="C51" s="29">
         <f>INDEX(y1st,6)+0.5</f>
@@ -3895,11 +4069,11 @@
       </c>
       <c r="D51" s="29">
         <f>INDEX(z1st,14)+Hght_WinWall2</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F51" s="28">
         <f>INDEX(x2nd,6)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="G51" s="29">
         <f>INDEX(y2nd,6)+0.5</f>
@@ -3907,11 +4081,11 @@
       </c>
       <c r="H51" s="29">
         <f>INDEX(z2nd,14)+Hght_WinWall2</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J51" s="28">
         <f>INDEX(x3rd,6)</f>
-        <v>12.9</v>
+        <v>7.24</v>
       </c>
       <c r="K51" s="29">
         <f>INDEX(y3rd,6)+0.5</f>
@@ -3919,11 +4093,11 @@
       </c>
       <c r="L51" s="29">
         <f>INDEX(z3rd,14)+Hght_WinWall2</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
       <c r="N51" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.62</v>
       </c>
       <c r="O51" s="24">
         <v>0</v>
@@ -3939,35 +4113,35 @@
       </c>
       <c r="B52" s="30">
         <f>INDEX(x1st,3)-0.5</f>
-        <v>12.4</v>
+        <v>6.74</v>
       </c>
       <c r="C52" s="31">
         <f>INDEX(y1st,3)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D52" s="31">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F52" s="30">
         <f>INDEX(x2nd,3)-0.5</f>
-        <v>12.4</v>
+        <v>6.74</v>
       </c>
       <c r="G52" s="31">
         <f>INDEX(y2nd,3)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H52" s="31">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J52" s="30">
         <f>INDEX(x3rd,3)-0.5</f>
-        <v>12.4</v>
+        <v>6.74</v>
       </c>
       <c r="K52" s="31">
         <f>INDEX(y3rd,3)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L52" s="31">
         <f>INDEX(z3rd,3)+0.5</f>
@@ -3975,11 +4149,11 @@
       </c>
       <c r="N52" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.62</v>
       </c>
       <c r="O52" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="P52" s="24">
         <f>+C32</f>
@@ -3992,35 +4166,35 @@
       </c>
       <c r="B53" s="30">
         <f>INDEX(x1st,17)-Len_WinWall3</f>
-        <v>5.95</v>
+        <v>3.12</v>
       </c>
       <c r="C53" s="31">
         <f>INDEX(y1st,4)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D53" s="31">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F53" s="30">
         <f>INDEX(x2nd,17)-Len_WinWall3</f>
-        <v>5.95</v>
+        <v>3.12</v>
       </c>
       <c r="G53" s="31">
         <f>INDEX(y2nd,4)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H53" s="31">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J53" s="30">
         <f>INDEX(x3rd,17)-Len_WinWall3</f>
-        <v>5.95</v>
+        <v>3.12</v>
       </c>
       <c r="K53" s="31">
         <f>INDEX(y3rd,4)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L53" s="31">
         <f>INDEX(z3rd,4)+0.5</f>
@@ -4033,39 +4207,39 @@
       </c>
       <c r="B54" s="30">
         <f>INDEX(x1st,18)</f>
-        <v>5.95</v>
+        <v>3.12</v>
       </c>
       <c r="C54" s="31">
         <f>INDEX(y1st,18)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D54" s="31">
         <f>INDEX(z1st,18)+Hght_WinWall3</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F54" s="30">
         <f>INDEX(x2nd,18)</f>
-        <v>5.95</v>
+        <v>3.12</v>
       </c>
       <c r="G54" s="31">
         <f>INDEX(y2nd,18)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H54" s="31">
         <f>INDEX(z2nd,18)+Hght_WinWall3</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J54" s="30">
         <f>INDEX(x3rd,18)</f>
-        <v>5.95</v>
+        <v>3.12</v>
       </c>
       <c r="K54" s="31">
         <f>INDEX(y3rd,18)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L54" s="31">
         <f>INDEX(z3rd,18)+Hght_WinWall3</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4074,39 +4248,39 @@
       </c>
       <c r="B55" s="30">
         <f>INDEX(x1st,17)</f>
-        <v>12.4</v>
+        <v>6.74</v>
       </c>
       <c r="C55" s="31">
         <f>INDEX(y1st,19)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="D55" s="31">
         <f>INDEX(z1st,19)</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F55" s="30">
         <f>INDEX(x2nd,17)</f>
-        <v>12.4</v>
+        <v>6.74</v>
       </c>
       <c r="G55" s="31">
         <f>INDEX(y2nd,19)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="H55" s="31">
         <f>INDEX(z2nd,19)</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J55" s="30">
         <f>INDEX(x3rd,17)</f>
-        <v>12.4</v>
+        <v>6.74</v>
       </c>
       <c r="K55" s="31">
         <f>INDEX(y3rd,19)</f>
-        <v>8.6344413705656891</v>
+        <v>12.348066298342541</v>
       </c>
       <c r="L55" s="31">
         <f>INDEX(z3rd,19)</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4119,11 +4293,11 @@
       </c>
       <c r="C56" s="32">
         <f>INDEX(y1st,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>11.848066298342541</v>
       </c>
       <c r="D56" s="32">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F56" s="32">
         <f>INDEX(x2nd,4)</f>
@@ -4131,11 +4305,11 @@
       </c>
       <c r="G56" s="32">
         <f>INDEX(y2nd,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>11.848066298342541</v>
       </c>
       <c r="H56" s="32">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J56" s="32">
         <f>INDEX(x3rd,4)</f>
@@ -4143,7 +4317,7 @@
       </c>
       <c r="K56" s="32">
         <f>INDEX(y3rd,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>11.848066298342541</v>
       </c>
       <c r="L56" s="32">
         <f>INDEX(z3rd,4)+0.5</f>
@@ -4160,11 +4334,11 @@
       </c>
       <c r="C57" s="32">
         <f>INDEX(y1st,21)-Len_WinWall4</f>
-        <v>7.27099723350912</v>
+        <v>10.613259668508288</v>
       </c>
       <c r="D57" s="32">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>3.09</v>
       </c>
       <c r="F57" s="32">
         <f>INDEX(x2nd,1)</f>
@@ -4172,11 +4346,11 @@
       </c>
       <c r="G57" s="32">
         <f>INDEX(y2nd,21)-Len_WinWall4</f>
-        <v>7.27099723350912</v>
+        <v>10.613259668508288</v>
       </c>
       <c r="H57" s="32">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="J57" s="32">
         <f>INDEX(x3rd,1)</f>
@@ -4184,7 +4358,7 @@
       </c>
       <c r="K57" s="32">
         <f>INDEX(y3rd,21)-Len_WinWall4</f>
-        <v>7.27099723350912</v>
+        <v>10.613259668508288</v>
       </c>
       <c r="L57" s="32">
         <f>INDEX(z3rd,1)+0.5</f>
@@ -4201,11 +4375,11 @@
       </c>
       <c r="C58" s="32">
         <f>INDEX(y1st,22)</f>
-        <v>7.27099723350912</v>
+        <v>10.613259668508288</v>
       </c>
       <c r="D58" s="32">
         <f>INDEX(z1st,22)+Hght_WinWall4</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F58" s="32">
         <f>INDEX(x2nd,5)</f>
@@ -4213,11 +4387,11 @@
       </c>
       <c r="G58" s="32">
         <f>INDEX(y2nd,22)</f>
-        <v>7.27099723350912</v>
+        <v>10.613259668508288</v>
       </c>
       <c r="H58" s="32">
         <f>INDEX(z2nd,22)+Hght_WinWall4</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J58" s="32">
         <f>INDEX(x3rd,5)</f>
@@ -4225,11 +4399,11 @@
       </c>
       <c r="K58" s="32">
         <f>INDEX(y3rd,22)</f>
-        <v>7.27099723350912</v>
+        <v>10.613259668508288</v>
       </c>
       <c r="L58" s="32">
         <f>INDEX(z3rd,22)+Hght_WinWall4</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4242,11 +4416,11 @@
       </c>
       <c r="C59" s="32">
         <f>INDEX(y1st,21)</f>
-        <v>8.1344413705656891</v>
+        <v>11.848066298342541</v>
       </c>
       <c r="D59" s="32">
         <f>INDEX(z1st,23)</f>
-        <v>4.3334000000000001</v>
+        <v>4.45</v>
       </c>
       <c r="F59" s="32">
         <f>INDEX(x2nd,8)</f>
@@ -4254,11 +4428,11 @@
       </c>
       <c r="G59" s="32">
         <f>INDEX(y2nd,21)</f>
-        <v>8.1344413705656891</v>
+        <v>11.848066298342541</v>
       </c>
       <c r="H59" s="32">
         <f>INDEX(z2nd,23)</f>
-        <v>7.1234000000000011</v>
+        <v>7.1700000000000008</v>
       </c>
       <c r="J59" s="32">
         <f>INDEX(x3rd,8)</f>
@@ -4266,11 +4440,11 @@
       </c>
       <c r="K59" s="32">
         <f>INDEX(y3rd,21)</f>
-        <v>8.1344413705656891</v>
+        <v>11.848066298342541</v>
       </c>
       <c r="L59" s="32">
         <f>INDEX(z3rd,23)</f>
-        <v>1.8950000000000002</v>
+        <v>1.8600000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4514,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="80" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G2" s="53" t="s">
         <v>133</v>
@@ -4407,15 +4581,15 @@
       </c>
       <c r="E7" s="55">
         <f>+main_area+second_area+third_area</f>
-        <v>193.98154031771418</v>
+        <v>182.91299476243097</v>
       </c>
       <c r="F7" s="55">
         <f>+E7*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>1968.8571843233306</v>
       </c>
       <c r="G7" s="81">
         <f>+D7*F7</f>
-        <v>19924.139978755939</v>
+        <v>18787.272776631959</v>
       </c>
       <c r="H7" t="s">
         <v>143</v>
@@ -4464,15 +4638,15 @@
       </c>
       <c r="E10" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>182.91299476243097</v>
       </c>
       <c r="F10" s="55">
         <f>+E10*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>1968.8571843233306</v>
       </c>
       <c r="G10" s="81">
         <f>+D10*F10</f>
-        <v>21835.818057760935</v>
+        <v>20589.870909834652</v>
       </c>
       <c r="H10" t="s">
         <v>144</v>
@@ -4521,18 +4695,18 @@
       </c>
       <c r="E13" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>182.91299476243097</v>
       </c>
       <c r="F13" s="55">
         <f>+E13*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>1968.8571843233306</v>
       </c>
       <c r="G13" s="81">
         <f>+D13*F13</f>
-        <v>19856.860046363774</v>
+        <v>18723.831822914872</v>
       </c>
       <c r="H13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -4578,15 +4752,15 @@
       </c>
       <c r="E16" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>182.91299476243097</v>
       </c>
       <c r="F16" s="55">
         <f>+E16*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>1968.8571843233306</v>
       </c>
       <c r="G16" s="81">
         <f t="shared" ref="G16:G17" si="0">+D16*F16</f>
-        <v>31319.968527387653</v>
+        <v>29532.857764849959</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -4602,15 +4776,15 @@
       </c>
       <c r="E17" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>182.91299476243097</v>
       </c>
       <c r="F17" s="55">
         <f>+E17*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>1968.8571843233306</v>
       </c>
       <c r="G17" s="81">
         <f t="shared" si="0"/>
-        <v>33522.806313813919</v>
+        <v>31610.002094311072</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4663,18 +4837,18 @@
       </c>
       <c r="E21" s="55">
         <f>found_wall_area</f>
-        <v>105.01916367597477</v>
+        <v>101.46618342541436</v>
       </c>
       <c r="F21" s="55">
         <f>+E21*10.7639</f>
-        <v>1130.4157758918248</v>
+        <v>1092.1718517728175</v>
       </c>
       <c r="G21" s="68">
         <f>+F21*D21</f>
-        <v>4928.6127828883555</v>
+        <v>4761.8692737294832</v>
       </c>
       <c r="H21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -4718,18 +4892,18 @@
       </c>
       <c r="E24" s="55">
         <f>found_wall_area</f>
-        <v>105.01916367597477</v>
+        <v>101.46618342541436</v>
       </c>
       <c r="F24" s="55">
         <f>+E24*10.7639</f>
-        <v>1130.4157758918248</v>
+        <v>1092.1718517728175</v>
       </c>
       <c r="G24" s="68">
         <f>+F24*D24</f>
-        <v>10060.700405437243</v>
+        <v>9720.3294807780785</v>
       </c>
       <c r="H24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -4754,18 +4928,18 @@
       </c>
       <c r="E26" s="55">
         <f>+Opt_Area</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="F26" s="55">
         <f>+E26*10.7639</f>
-        <v>1198.929398745353</v>
+        <v>962.29266000000007</v>
       </c>
       <c r="G26" s="68">
         <f>+F26*D26</f>
-        <v>1103.0150468457248</v>
+        <v>885.30924720000007</v>
       </c>
       <c r="H26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -4781,18 +4955,18 @@
       </c>
       <c r="E27" s="55">
         <f>+Opt_Area</f>
-        <v>111.38429368029739</v>
+        <v>89.4</v>
       </c>
       <c r="F27" s="55">
         <f>+E27*10.7639</f>
-        <v>1198.929398745353</v>
+        <v>962.29266000000007</v>
       </c>
       <c r="G27" s="68">
         <f>+F27*D27</f>
-        <v>1198.929398745353</v>
+        <v>962.29266000000007</v>
       </c>
       <c r="H27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -4905,10 +5079,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="47" t="s">
         <v>164</v>
-      </c>
-      <c r="C37" s="47" t="s">
-        <v>165</v>
       </c>
       <c r="D37" s="81">
         <f>+'[1]UNIT COSTS'!$H$63</f>
@@ -4916,23 +5090,23 @@
       </c>
       <c r="E37" s="47">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>20.019372088397791</v>
       </c>
       <c r="F37" s="55">
         <f t="shared" ref="F37:F40" si="1">+E37*10.7639</f>
-        <v>336.57333665604727</v>
+        <v>215.48651922230496</v>
       </c>
       <c r="G37" s="68">
         <f>+D37*F37</f>
-        <v>23760.981397166746</v>
+        <v>15212.646448621786</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D38" s="81">
         <f>+'[1]UNIT COSTS'!$H$64</f>
@@ -4940,23 +5114,23 @@
       </c>
       <c r="E38" s="89">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>20.019372088397791</v>
       </c>
       <c r="F38" s="55">
         <f t="shared" si="1"/>
-        <v>336.57333665604727</v>
+        <v>215.48651922230496</v>
       </c>
       <c r="G38" s="68">
         <f t="shared" ref="G38:G40" si="2">+D38*F38</f>
-        <v>23760.981397166746</v>
+        <v>15212.646448621786</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D39" s="81">
         <f>+'[1]UNIT COSTS'!$H$65</f>
@@ -4964,23 +5138,23 @@
       </c>
       <c r="E39" s="89">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>20.019372088397791</v>
       </c>
       <c r="F39" s="55">
         <f t="shared" si="1"/>
-        <v>336.57333665604727</v>
+        <v>215.48651922230496</v>
       </c>
       <c r="G39" s="68">
         <f t="shared" si="2"/>
-        <v>26538.405165588203</v>
+        <v>16990.854390488723</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D40" s="81">
         <f>+'[1]UNIT COSTS'!$H$66</f>
@@ -4988,15 +5162,15 @@
       </c>
       <c r="E40" s="89">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>20.019372088397791</v>
       </c>
       <c r="F40" s="55">
         <f t="shared" si="1"/>
-        <v>336.57333665604727</v>
+        <v>215.48651922230496</v>
       </c>
       <c r="G40" s="68">
         <f t="shared" si="2"/>
-        <v>26538.405165588203</v>
+        <v>16990.854390488723</v>
       </c>
     </row>
   </sheetData>
@@ -5080,11 +5254,11 @@
       <c r="H3" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -5674,21 +5848,21 @@
       <c r="C25" s="61"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="96" t="s">
+      <c r="B26" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="F26" s="96" t="s">
+      <c r="C26" s="101"/>
+      <c r="D26" s="101"/>
+      <c r="F26" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="G26" s="96"/>
-      <c r="H26" s="96"/>
-      <c r="J26" s="96" t="s">
+      <c r="G26" s="101"/>
+      <c r="H26" s="101"/>
+      <c r="J26" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="96"/>
-      <c r="L26" s="96"/>
+      <c r="K26" s="101"/>
+      <c r="L26" s="101"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">

</xml_diff>